<commit_message>
Added LD instruction to Control Unit microcode
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="773"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="773"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
   <si>
     <t>NextAddressSource</t>
   </si>
@@ -28,18 +28,6 @@
     <t>Microinstruction</t>
   </si>
   <si>
-    <t>0x0000</t>
-  </si>
-  <si>
-    <t>0x0001</t>
-  </si>
-  <si>
-    <t>0x0002</t>
-  </si>
-  <si>
-    <t>0x0003</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -220,44 +208,83 @@
     <t>010: SgnExt IR[Offset]</t>
   </si>
   <si>
-    <t>011: Constant 0</t>
-  </si>
-  <si>
     <t>111: Random signed 32bit</t>
   </si>
   <si>
-    <t>100: UNUSED/RESERVED</t>
-  </si>
-  <si>
     <t>101: UNUSED/RESERVED</t>
   </si>
   <si>
     <t>110: UNUSED/RESERVED</t>
   </si>
   <si>
-    <t>(10 bit)</t>
-  </si>
-  <si>
-    <t>0000000000</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>MAR_LD</t>
+  </si>
+  <si>
+    <t>1: MAR Write</t>
+  </si>
+  <si>
+    <t>0: MAR Read</t>
+  </si>
+  <si>
+    <t>(8 bit)</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>Hlt</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>OpCode</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>00</t>
+    <t>Ld</t>
+  </si>
+  <si>
+    <t>100: Constant 0</t>
+  </si>
+  <si>
+    <t>011: ZeroExt IR[Address]</t>
+  </si>
+  <si>
+    <t>00000011</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>00000101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +298,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -294,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -313,12 +349,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -328,6 +384,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -633,197 +705,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U145"/>
+  <dimension ref="A1:W146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" customWidth="1"/>
+    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" customWidth="1"/>
+    <col min="22" max="23" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="6" t="s">
+    <row r="1" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="6" t="s">
+      <c r="P6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="V8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W8" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -831,72 +912,78 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="T9" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>1</v>
       </c>
       <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>73</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
       </c>
       <c r="I10" t="s">
         <v>1</v>
@@ -905,22 +992,22 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="O10" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="P10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="Q10" t="s">
         <v>1</v>
@@ -934,185 +1021,440 @@
       <c r="T10" t="s">
         <v>1</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="V10" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>0</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10" t="str">
+        <f>CONCATENATE(F11,G11,H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11,V11,W11)</f>
+        <v>00000000010000000000000001001100</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10" t="str">
+        <f>CONCATENATE(F12,G12,H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,U12,V12,W12)</f>
+        <v>00000000101000000000000000000001</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="W12" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15" t="str">
+        <f>CONCATENATE(F13,G13,H13,I13,J13,K13,L13,M13,N13,O13,P13,Q13,R13,S13,T13,U13,V13,W13)</f>
+        <v>10000000000000000000000000000000</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="W13" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>3</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19" t="str">
+        <f>CONCATENATE(F14,G14,H14,I14,J14,K14,L14,M14,N14,O14,P14,Q14,R14,S14,T14,U14,V14,W14)</f>
+        <v>00000000110000000000000000000000</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="T14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="W14" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
         <v>4</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7" t="str">
-        <f>CONCATENATE(F11,G11,H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11)</f>
-        <v>10000000000000000000000000000001</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="B15" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f t="shared" ref="D15:D27" si="0">CONCATENATE(F15,G15,H15,I15,J15,K15,L15,M15,N15,O15,P15,Q15,R15,S15,T15,U15,V15,W15)</f>
+        <v>00000001010000111000000000100100</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000000010000000000000000001</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="I16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
         <v>6</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-    </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1130,8 +1472,17 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-    </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>7</v>
+      </c>
+      <c r="D18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1149,8 +1500,14 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-    </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1168,8 +1525,14 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-    </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D20" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1187,8 +1550,15 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D21" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1205,8 +1575,15 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D22" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1223,8 +1600,15 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D23" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1241,8 +1625,15 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D24" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1259,8 +1650,15 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-    </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1277,8 +1675,15 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1295,8 +1700,15 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1313,8 +1725,11 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1331,8 +1746,11 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1349,8 +1767,11 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1367,8 +1788,11 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-    </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1385,11 +1809,12 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -1403,11 +1828,12 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -1421,11 +1847,12 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
-    </row>
-    <row r="34" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -1439,11 +1866,12 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -1457,11 +1885,12 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -1475,11 +1904,12 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+    </row>
+    <row r="37" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -1493,11 +1923,12 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-    </row>
-    <row r="38" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -1511,11 +1942,12 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-    </row>
-    <row r="39" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+    </row>
+    <row r="39" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -1529,11 +1961,12 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
-    </row>
-    <row r="40" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -1547,11 +1980,12 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-    </row>
-    <row r="41" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+    </row>
+    <row r="41" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -1565,11 +1999,12 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+    </row>
+    <row r="42" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -1583,11 +2018,12 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+    </row>
+    <row r="43" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -1601,11 +2037,12 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+    </row>
+    <row r="44" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -1619,11 +2056,12 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -1637,11 +2075,12 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -1655,11 +2094,12 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-    </row>
-    <row r="47" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -1673,11 +2113,12 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-    </row>
-    <row r="48" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -1691,11 +2132,12 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
-    </row>
-    <row r="49" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+    </row>
+    <row r="49" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -1709,11 +2151,12 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
-    </row>
-    <row r="50" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -1727,11 +2170,12 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
-    </row>
-    <row r="51" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+    </row>
+    <row r="51" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -1745,11 +2189,12 @@
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
-    </row>
-    <row r="52" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+    </row>
+    <row r="52" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -1763,11 +2208,12 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+    </row>
+    <row r="53" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -1781,11 +2227,12 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
-    </row>
-    <row r="54" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+    </row>
+    <row r="54" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -1799,11 +2246,12 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
-    </row>
-    <row r="55" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+    </row>
+    <row r="55" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -1817,11 +2265,12 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
-    </row>
-    <row r="56" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+    </row>
+    <row r="56" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -1835,11 +2284,12 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-    </row>
-    <row r="57" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+    </row>
+    <row r="57" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -1853,11 +2303,12 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
-    </row>
-    <row r="58" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+    </row>
+    <row r="58" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -1871,11 +2322,12 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-    </row>
-    <row r="59" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+    </row>
+    <row r="59" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -1889,11 +2341,12 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
-    </row>
-    <row r="60" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+    </row>
+    <row r="60" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -1907,11 +2360,12 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
-    </row>
-    <row r="61" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V60" s="2"/>
+      <c r="W60" s="2"/>
+    </row>
+    <row r="61" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -1925,11 +2379,12 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-    </row>
-    <row r="62" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+    </row>
+    <row r="62" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -1943,11 +2398,12 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-    </row>
-    <row r="63" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V62" s="2"/>
+      <c r="W62" s="2"/>
+    </row>
+    <row r="63" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -1961,11 +2417,12 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-    </row>
-    <row r="64" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V63" s="2"/>
+      <c r="W63" s="2"/>
+    </row>
+    <row r="64" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -1979,11 +2436,12 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
-    </row>
-    <row r="65" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V64" s="2"/>
+      <c r="W64" s="2"/>
+    </row>
+    <row r="65" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -1997,11 +2455,12 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
-    </row>
-    <row r="66" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V65" s="2"/>
+      <c r="W65" s="2"/>
+    </row>
+    <row r="66" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -2015,11 +2474,12 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
-    </row>
-    <row r="67" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V66" s="2"/>
+      <c r="W66" s="2"/>
+    </row>
+    <row r="67" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -2033,11 +2493,12 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
-    </row>
-    <row r="68" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V67" s="2"/>
+      <c r="W67" s="2"/>
+    </row>
+    <row r="68" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -2051,11 +2512,12 @@
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
-    </row>
-    <row r="69" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+    </row>
+    <row r="69" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -2069,11 +2531,12 @@
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
-    </row>
-    <row r="70" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+    </row>
+    <row r="70" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -2087,11 +2550,12 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
-    </row>
-    <row r="71" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V70" s="2"/>
+      <c r="W70" s="2"/>
+    </row>
+    <row r="71" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -2105,11 +2569,12 @@
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
-    </row>
-    <row r="72" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+    </row>
+    <row r="72" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -2123,11 +2588,12 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
-    </row>
-    <row r="73" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V72" s="2"/>
+      <c r="W72" s="2"/>
+    </row>
+    <row r="73" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -2141,11 +2607,12 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-    </row>
-    <row r="74" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V73" s="2"/>
+      <c r="W73" s="2"/>
+    </row>
+    <row r="74" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
@@ -2159,11 +2626,12 @@
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-    </row>
-    <row r="75" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V74" s="2"/>
+      <c r="W74" s="2"/>
+    </row>
+    <row r="75" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -2177,11 +2645,12 @@
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-    </row>
-    <row r="76" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V75" s="2"/>
+      <c r="W75" s="2"/>
+    </row>
+    <row r="76" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -2195,11 +2664,12 @@
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-    </row>
-    <row r="77" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V76" s="2"/>
+      <c r="W76" s="2"/>
+    </row>
+    <row r="77" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -2213,11 +2683,12 @@
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
-    </row>
-    <row r="78" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V77" s="2"/>
+      <c r="W77" s="2"/>
+    </row>
+    <row r="78" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -2231,11 +2702,12 @@
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-    </row>
-    <row r="79" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V78" s="2"/>
+      <c r="W78" s="2"/>
+    </row>
+    <row r="79" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -2249,11 +2721,12 @@
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
-    </row>
-    <row r="80" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V79" s="2"/>
+      <c r="W79" s="2"/>
+    </row>
+    <row r="80" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -2267,11 +2740,12 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
-    </row>
-    <row r="81" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V80" s="2"/>
+      <c r="W80" s="2"/>
+    </row>
+    <row r="81" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
@@ -2285,11 +2759,12 @@
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
       <c r="U81" s="2"/>
-    </row>
-    <row r="82" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V81" s="2"/>
+      <c r="W81" s="2"/>
+    </row>
+    <row r="82" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -2303,11 +2778,12 @@
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
       <c r="U82" s="2"/>
-    </row>
-    <row r="83" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V82" s="2"/>
+      <c r="W82" s="2"/>
+    </row>
+    <row r="83" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -2321,11 +2797,12 @@
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
       <c r="U83" s="2"/>
-    </row>
-    <row r="84" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V83" s="2"/>
+      <c r="W83" s="2"/>
+    </row>
+    <row r="84" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -2339,11 +2816,12 @@
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
       <c r="U84" s="2"/>
-    </row>
-    <row r="85" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V84" s="2"/>
+      <c r="W84" s="2"/>
+    </row>
+    <row r="85" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -2357,11 +2835,12 @@
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
       <c r="U85" s="2"/>
-    </row>
-    <row r="86" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V85" s="2"/>
+      <c r="W85" s="2"/>
+    </row>
+    <row r="86" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -2375,11 +2854,12 @@
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
       <c r="U86" s="2"/>
-    </row>
-    <row r="87" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V86" s="2"/>
+      <c r="W86" s="2"/>
+    </row>
+    <row r="87" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
@@ -2393,11 +2873,12 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
       <c r="U87" s="2"/>
-    </row>
-    <row r="88" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V87" s="2"/>
+      <c r="W87" s="2"/>
+    </row>
+    <row r="88" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
@@ -2411,11 +2892,12 @@
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
       <c r="U88" s="2"/>
-    </row>
-    <row r="89" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V88" s="2"/>
+      <c r="W88" s="2"/>
+    </row>
+    <row r="89" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
@@ -2429,11 +2911,12 @@
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
-    </row>
-    <row r="90" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V89" s="2"/>
+      <c r="W89" s="2"/>
+    </row>
+    <row r="90" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -2447,11 +2930,12 @@
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
       <c r="U90" s="2"/>
-    </row>
-    <row r="91" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V90" s="2"/>
+      <c r="W90" s="2"/>
+    </row>
+    <row r="91" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -2465,11 +2949,12 @@
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
       <c r="U91" s="2"/>
-    </row>
-    <row r="92" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V91" s="2"/>
+      <c r="W91" s="2"/>
+    </row>
+    <row r="92" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -2483,11 +2968,12 @@
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
       <c r="U92" s="2"/>
-    </row>
-    <row r="93" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V92" s="2"/>
+      <c r="W92" s="2"/>
+    </row>
+    <row r="93" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
@@ -2501,11 +2987,12 @@
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
       <c r="U93" s="2"/>
-    </row>
-    <row r="94" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V93" s="2"/>
+      <c r="W93" s="2"/>
+    </row>
+    <row r="94" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -2519,11 +3006,12 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
       <c r="U94" s="2"/>
-    </row>
-    <row r="95" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V94" s="2"/>
+      <c r="W94" s="2"/>
+    </row>
+    <row r="95" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -2537,11 +3025,12 @@
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
       <c r="U95" s="2"/>
-    </row>
-    <row r="96" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V95" s="2"/>
+      <c r="W95" s="2"/>
+    </row>
+    <row r="96" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -2555,11 +3044,12 @@
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
       <c r="U96" s="2"/>
-    </row>
-    <row r="97" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V96" s="2"/>
+      <c r="W96" s="2"/>
+    </row>
+    <row r="97" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -2573,11 +3063,12 @@
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
       <c r="U97" s="2"/>
-    </row>
-    <row r="98" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V97" s="2"/>
+      <c r="W97" s="2"/>
+    </row>
+    <row r="98" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -2591,11 +3082,12 @@
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
       <c r="U98" s="2"/>
-    </row>
-    <row r="99" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V98" s="2"/>
+      <c r="W98" s="2"/>
+    </row>
+    <row r="99" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -2609,11 +3101,12 @@
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
       <c r="U99" s="2"/>
-    </row>
-    <row r="100" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V99" s="2"/>
+      <c r="W99" s="2"/>
+    </row>
+    <row r="100" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -2627,11 +3120,12 @@
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
       <c r="U100" s="2"/>
-    </row>
-    <row r="101" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V100" s="2"/>
+      <c r="W100" s="2"/>
+    </row>
+    <row r="101" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -2645,11 +3139,12 @@
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
       <c r="U101" s="2"/>
-    </row>
-    <row r="102" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V101" s="2"/>
+      <c r="W101" s="2"/>
+    </row>
+    <row r="102" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
@@ -2663,11 +3158,12 @@
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
       <c r="U102" s="2"/>
-    </row>
-    <row r="103" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V102" s="2"/>
+      <c r="W102" s="2"/>
+    </row>
+    <row r="103" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
@@ -2681,11 +3177,12 @@
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
       <c r="U103" s="2"/>
-    </row>
-    <row r="104" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V103" s="2"/>
+      <c r="W103" s="2"/>
+    </row>
+    <row r="104" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
@@ -2699,11 +3196,12 @@
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
       <c r="U104" s="2"/>
-    </row>
-    <row r="105" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V104" s="2"/>
+      <c r="W104" s="2"/>
+    </row>
+    <row r="105" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
@@ -2717,11 +3215,12 @@
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
       <c r="U105" s="2"/>
-    </row>
-    <row r="106" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V105" s="2"/>
+      <c r="W105" s="2"/>
+    </row>
+    <row r="106" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -2735,11 +3234,12 @@
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
       <c r="U106" s="2"/>
-    </row>
-    <row r="107" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V106" s="2"/>
+      <c r="W106" s="2"/>
+    </row>
+    <row r="107" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -2753,11 +3253,12 @@
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
       <c r="U107" s="2"/>
-    </row>
-    <row r="108" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V107" s="2"/>
+      <c r="W107" s="2"/>
+    </row>
+    <row r="108" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -2771,11 +3272,12 @@
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
       <c r="U108" s="2"/>
-    </row>
-    <row r="109" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V108" s="2"/>
+      <c r="W108" s="2"/>
+    </row>
+    <row r="109" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -2789,11 +3291,12 @@
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
       <c r="U109" s="2"/>
-    </row>
-    <row r="110" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V109" s="2"/>
+      <c r="W109" s="2"/>
+    </row>
+    <row r="110" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -2807,11 +3310,12 @@
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
-    </row>
-    <row r="111" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V110" s="2"/>
+      <c r="W110" s="2"/>
+    </row>
+    <row r="111" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -2825,11 +3329,12 @@
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
       <c r="U111" s="2"/>
-    </row>
-    <row r="112" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V111" s="2"/>
+      <c r="W111" s="2"/>
+    </row>
+    <row r="112" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -2843,11 +3348,12 @@
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
       <c r="U112" s="2"/>
-    </row>
-    <row r="113" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+    </row>
+    <row r="113" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
@@ -2861,11 +3367,12 @@
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
       <c r="U113" s="2"/>
-    </row>
-    <row r="114" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V113" s="2"/>
+      <c r="W113" s="2"/>
+    </row>
+    <row r="114" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -2879,11 +3386,12 @@
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
       <c r="U114" s="2"/>
-    </row>
-    <row r="115" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V114" s="2"/>
+      <c r="W114" s="2"/>
+    </row>
+    <row r="115" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -2897,11 +3405,12 @@
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
       <c r="U115" s="2"/>
-    </row>
-    <row r="116" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V115" s="2"/>
+      <c r="W115" s="2"/>
+    </row>
+    <row r="116" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
@@ -2915,11 +3424,12 @@
       <c r="S116" s="2"/>
       <c r="T116" s="2"/>
       <c r="U116" s="2"/>
-    </row>
-    <row r="117" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V116" s="2"/>
+      <c r="W116" s="2"/>
+    </row>
+    <row r="117" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
@@ -2933,11 +3443,12 @@
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
-    </row>
-    <row r="118" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V117" s="2"/>
+      <c r="W117" s="2"/>
+    </row>
+    <row r="118" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
@@ -2951,11 +3462,12 @@
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
       <c r="U118" s="2"/>
-    </row>
-    <row r="119" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V118" s="2"/>
+      <c r="W118" s="2"/>
+    </row>
+    <row r="119" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
@@ -2969,11 +3481,12 @@
       <c r="S119" s="2"/>
       <c r="T119" s="2"/>
       <c r="U119" s="2"/>
-    </row>
-    <row r="120" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V119" s="2"/>
+      <c r="W119" s="2"/>
+    </row>
+    <row r="120" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
@@ -2987,11 +3500,12 @@
       <c r="S120" s="2"/>
       <c r="T120" s="2"/>
       <c r="U120" s="2"/>
-    </row>
-    <row r="121" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V120" s="2"/>
+      <c r="W120" s="2"/>
+    </row>
+    <row r="121" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
@@ -3005,11 +3519,12 @@
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
       <c r="U121" s="2"/>
-    </row>
-    <row r="122" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V121" s="2"/>
+      <c r="W121" s="2"/>
+    </row>
+    <row r="122" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -3023,11 +3538,12 @@
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
-    </row>
-    <row r="123" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V122" s="2"/>
+      <c r="W122" s="2"/>
+    </row>
+    <row r="123" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -3041,11 +3557,12 @@
       <c r="S123" s="2"/>
       <c r="T123" s="2"/>
       <c r="U123" s="2"/>
-    </row>
-    <row r="124" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V123" s="2"/>
+      <c r="W123" s="2"/>
+    </row>
+    <row r="124" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -3059,11 +3576,12 @@
       <c r="S124" s="2"/>
       <c r="T124" s="2"/>
       <c r="U124" s="2"/>
-    </row>
-    <row r="125" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V124" s="2"/>
+      <c r="W124" s="2"/>
+    </row>
+    <row r="125" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
@@ -3077,11 +3595,12 @@
       <c r="S125" s="2"/>
       <c r="T125" s="2"/>
       <c r="U125" s="2"/>
-    </row>
-    <row r="126" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V125" s="2"/>
+      <c r="W125" s="2"/>
+    </row>
+    <row r="126" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
@@ -3095,11 +3614,12 @@
       <c r="S126" s="2"/>
       <c r="T126" s="2"/>
       <c r="U126" s="2"/>
-    </row>
-    <row r="127" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V126" s="2"/>
+      <c r="W126" s="2"/>
+    </row>
+    <row r="127" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
       <c r="I127" s="2"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
@@ -3113,11 +3633,12 @@
       <c r="S127" s="2"/>
       <c r="T127" s="2"/>
       <c r="U127" s="2"/>
-    </row>
-    <row r="128" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V127" s="2"/>
+      <c r="W127" s="2"/>
+    </row>
+    <row r="128" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
@@ -3131,11 +3652,12 @@
       <c r="S128" s="2"/>
       <c r="T128" s="2"/>
       <c r="U128" s="2"/>
-    </row>
-    <row r="129" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V128" s="2"/>
+      <c r="W128" s="2"/>
+    </row>
+    <row r="129" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
@@ -3149,11 +3671,12 @@
       <c r="S129" s="2"/>
       <c r="T129" s="2"/>
       <c r="U129" s="2"/>
-    </row>
-    <row r="130" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V129" s="2"/>
+      <c r="W129" s="2"/>
+    </row>
+    <row r="130" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
       <c r="I130" s="2"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
@@ -3167,11 +3690,12 @@
       <c r="S130" s="2"/>
       <c r="T130" s="2"/>
       <c r="U130" s="2"/>
-    </row>
-    <row r="131" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V130" s="2"/>
+      <c r="W130" s="2"/>
+    </row>
+    <row r="131" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
       <c r="I131" s="2"/>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
@@ -3185,11 +3709,12 @@
       <c r="S131" s="2"/>
       <c r="T131" s="2"/>
       <c r="U131" s="2"/>
-    </row>
-    <row r="132" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V131" s="2"/>
+      <c r="W131" s="2"/>
+    </row>
+    <row r="132" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -3203,11 +3728,12 @@
       <c r="S132" s="2"/>
       <c r="T132" s="2"/>
       <c r="U132" s="2"/>
-    </row>
-    <row r="133" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V132" s="2"/>
+      <c r="W132" s="2"/>
+    </row>
+    <row r="133" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
@@ -3221,11 +3747,12 @@
       <c r="S133" s="2"/>
       <c r="T133" s="2"/>
       <c r="U133" s="2"/>
-    </row>
-    <row r="134" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V133" s="2"/>
+      <c r="W133" s="2"/>
+    </row>
+    <row r="134" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
@@ -3239,11 +3766,12 @@
       <c r="S134" s="2"/>
       <c r="T134" s="2"/>
       <c r="U134" s="2"/>
-    </row>
-    <row r="135" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V134" s="2"/>
+      <c r="W134" s="2"/>
+    </row>
+    <row r="135" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
       <c r="I135" s="2"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -3257,11 +3785,12 @@
       <c r="S135" s="2"/>
       <c r="T135" s="2"/>
       <c r="U135" s="2"/>
-    </row>
-    <row r="136" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V135" s="2"/>
+      <c r="W135" s="2"/>
+    </row>
+    <row r="136" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
@@ -3275,11 +3804,12 @@
       <c r="S136" s="2"/>
       <c r="T136" s="2"/>
       <c r="U136" s="2"/>
-    </row>
-    <row r="137" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V136" s="2"/>
+      <c r="W136" s="2"/>
+    </row>
+    <row r="137" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
@@ -3293,11 +3823,12 @@
       <c r="S137" s="2"/>
       <c r="T137" s="2"/>
       <c r="U137" s="2"/>
-    </row>
-    <row r="138" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V137" s="2"/>
+      <c r="W137" s="2"/>
+    </row>
+    <row r="138" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
@@ -3311,11 +3842,12 @@
       <c r="S138" s="2"/>
       <c r="T138" s="2"/>
       <c r="U138" s="2"/>
-    </row>
-    <row r="139" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V138" s="2"/>
+      <c r="W138" s="2"/>
+    </row>
+    <row r="139" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
       <c r="I139" s="2"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
@@ -3329,11 +3861,12 @@
       <c r="S139" s="2"/>
       <c r="T139" s="2"/>
       <c r="U139" s="2"/>
-    </row>
-    <row r="140" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V139" s="2"/>
+      <c r="W139" s="2"/>
+    </row>
+    <row r="140" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
@@ -3347,11 +3880,12 @@
       <c r="S140" s="2"/>
       <c r="T140" s="2"/>
       <c r="U140" s="2"/>
-    </row>
-    <row r="141" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V140" s="2"/>
+      <c r="W140" s="2"/>
+    </row>
+    <row r="141" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
@@ -3365,11 +3899,12 @@
       <c r="S141" s="2"/>
       <c r="T141" s="2"/>
       <c r="U141" s="2"/>
-    </row>
-    <row r="142" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V141" s="2"/>
+      <c r="W141" s="2"/>
+    </row>
+    <row r="142" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
@@ -3383,11 +3918,12 @@
       <c r="S142" s="2"/>
       <c r="T142" s="2"/>
       <c r="U142" s="2"/>
-    </row>
-    <row r="143" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V142" s="2"/>
+      <c r="W142" s="2"/>
+    </row>
+    <row r="143" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
@@ -3401,11 +3937,12 @@
       <c r="S143" s="2"/>
       <c r="T143" s="2"/>
       <c r="U143" s="2"/>
-    </row>
-    <row r="144" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V143" s="2"/>
+      <c r="W143" s="2"/>
+    </row>
+    <row r="144" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
@@ -3419,11 +3956,12 @@
       <c r="S144" s="2"/>
       <c r="T144" s="2"/>
       <c r="U144" s="2"/>
-    </row>
-    <row r="145" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="V144" s="2"/>
+      <c r="W144" s="2"/>
+    </row>
+    <row r="145" spans="6:23" x14ac:dyDescent="0.3">
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
       <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
@@ -3437,8 +3975,30 @@
       <c r="S145" s="2"/>
       <c r="T145" s="2"/>
       <c r="U145" s="2"/>
+      <c r="V145" s="2"/>
+      <c r="W145" s="2"/>
+    </row>
+    <row r="146" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
+      <c r="R146" s="2"/>
+      <c r="S146" s="2"/>
+      <c r="T146" s="2"/>
+      <c r="U146" s="2"/>
+      <c r="V146" s="2"/>
+      <c r="W146" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ST instruction to CU uCode
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="86">
   <si>
     <t>NextAddressSource</t>
   </si>
@@ -25,9 +25,6 @@
     <t>ROM Address</t>
   </si>
   <si>
-    <t>Microinstruction</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -238,18 +235,9 @@
     <t>(8 bit)</t>
   </si>
   <si>
-    <t>00000000</t>
-  </si>
-  <si>
-    <t>00000001</t>
-  </si>
-  <si>
     <t>Hlt</t>
   </si>
   <si>
-    <t>00000010</t>
-  </si>
-  <si>
     <t>OpCode</t>
   </si>
   <si>
@@ -265,9 +253,6 @@
     <t>011: ZeroExt IR[Address]</t>
   </si>
   <si>
-    <t>00000011</t>
-  </si>
-  <si>
     <t>011</t>
   </si>
   <si>
@@ -277,7 +262,16 @@
     <t>2</t>
   </si>
   <si>
-    <t>00000101</t>
+    <t>St</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -330,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -369,16 +363,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -400,6 +439,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -705,288 +754,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W146"/>
+  <dimension ref="A1:X146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" customWidth="1"/>
-    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5546875" customWidth="1"/>
-    <col min="22" max="23" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5546875" customWidth="1"/>
+    <col min="23" max="24" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L1" s="6" t="s">
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="25"/>
+      <c r="M1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="25"/>
+      <c r="M2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="25"/>
+      <c r="M3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="25"/>
+      <c r="M4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="25"/>
+      <c r="M5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="25"/>
+      <c r="M6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="25"/>
+      <c r="G7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="25"/>
+      <c r="G8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="Q9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="R7" s="6" t="s">
+      <c r="S9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="U9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="T7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="V7" s="6" t="s">
+      <c r="V9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W7" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G10" t="s">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="J10" t="s">
         <v>1</v>
@@ -995,22 +1051,22 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="N10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="Q10" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="R10" t="s">
         <v>1</v>
@@ -1021,340 +1077,365 @@
       <c r="T10" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="U10" t="s">
         <v>1</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="W10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="X10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>0</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10" t="str">
-        <f>CONCATENATE(F11,G11,H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11,V11,W11)</f>
+      <c r="B11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9" t="str">
+        <f>CONCATENATE(G11,H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11,V11,W11,X11)</f>
         <v>00000000010000000000000001001100</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="28" t="str">
+        <f>CONCATENATE(BIN2HEX(VALUE(MID(D11,1, 4))),BIN2HEX(VALUE(MID(D11,5, 4))),BIN2HEX(VALUE(MID(D11,9, 4))),BIN2HEX(VALUE(MID(D11,13, 4))),BIN2HEX(VALUE(MID(D11,17, 4))),BIN2HEX(VALUE(MID(D11,21, 4))),BIN2HEX(VALUE(MID(D11,25, 4))),BIN2HEX(VALUE(MID(D11,29, 4))))</f>
+        <v>0040004C</v>
+      </c>
+      <c r="F11" s="10">
         <v>0</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="31" t="str">
+        <f>DEC2BIN(A12,8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="N11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q11" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="R11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="S11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="str">
+        <f>CONCATENATE(G12,H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,U12,V12,W12,X12)</f>
+        <v>00000000101000000000000000000001</v>
+      </c>
+      <c r="E12" s="28" t="str">
+        <f t="shared" ref="E12:E30" si="0">CONCATENATE(BIN2HEX(VALUE(MID(D12,1, 4))),BIN2HEX(VALUE(MID(D12,5, 4))),BIN2HEX(VALUE(MID(D12,9, 4))),BIN2HEX(VALUE(MID(D12,13, 4))),BIN2HEX(VALUE(MID(D12,17, 4))),BIN2HEX(VALUE(MID(D12,21, 4))),BIN2HEX(VALUE(MID(D12,25, 4))),BIN2HEX(VALUE(MID(D12,29, 4))))</f>
+        <v>00A00001</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="31" t="str">
+        <f>DEC2BIN(A13,8)</f>
+        <v>00000010</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="N12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="R12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="X12" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14" t="str">
+        <f>CONCATENATE(G13,H13,I13,J13,K13,L13,M13,N13,O13,P13,Q13,R13,S13,T13,U13,V13,W13,X13)</f>
+        <v>10000000000000000000000000000000</v>
+      </c>
+      <c r="E13" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>80000000</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="32" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="N13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="P11" s="11" t="s">
+      <c r="O13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="P13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="X13" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
+        <v>3</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18" t="str">
+        <f>CONCATENATE(G14,H14,I14,J14,K14,L14,M14,N14,O14,P14,Q14,R14,S14,T14,U14,V14,W14,X14)</f>
+        <v>00000000110000000000000000000000</v>
+      </c>
+      <c r="E14" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>00C00000</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="33" t="str">
+        <f>DEC2BIN($A$14,8)</f>
+        <v>00000011</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="V14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="W14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="X14" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>4</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f>CONCATENATE(G15,H15,I15,J15,K15,L15,M15,N15,O15,P15,Q15,R15,S15,T15,U15,V15,W15,X15)</f>
+        <v>00000001010000111000000000100100</v>
+      </c>
+      <c r="E15" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>01438024</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="31" t="str">
+        <f>DEC2BIN(A16,8)</f>
+        <v>00000101</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="S11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="T11" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="V11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="W11" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10" t="str">
-        <f>CONCATENATE(F12,G12,H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,U12,V12,W12)</f>
-        <v>00000000101000000000000000000001</v>
-      </c>
-      <c r="E12" s="11">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="N15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="P12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="S12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="W12" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>2</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15" t="str">
-        <f>CONCATENATE(F13,G13,H13,I13,J13,K13,L13,M13,N13,O13,P13,Q13,R13,S13,T13,U13,V13,W13)</f>
-        <v>10000000000000000000000000000000</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="S13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="U13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="W13" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>3</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="18">
-        <v>0</v>
-      </c>
-      <c r="D14" s="19" t="str">
-        <f>CONCATENATE(F14,G14,H14,I14,J14,K14,L14,M14,N14,O14,P14,Q14,R14,S14,T14,U14,V14,W14)</f>
-        <v>00000000110000000000000000000000</v>
-      </c>
-      <c r="E14" s="20">
-        <v>0</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="P14" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="S14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="T14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="U14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="V14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="W14" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>4</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f t="shared" ref="D15:D27" si="0">CONCATENATE(F15,G15,H15,I15,J15,K15,L15,M15,N15,O15,P15,Q15,R15,S15,T15,U15,V15,W15)</f>
-        <v>00000001010000111000000000100100</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>68</v>
@@ -1363,152 +1444,260 @@
         <v>67</v>
       </c>
       <c r="R15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>5</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14" t="str">
+        <f>CONCATENATE(G16,H16,I16,J16,K16,L16,M16,N16,O16,P16,Q16,R16,S16,T16,U16,V16,W16,X16)</f>
+        <v>00000000000010000000000000000001</v>
+      </c>
+      <c r="E16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>00080001</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="32" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="V16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="W16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="X16" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>6</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f>CONCATENATE(G17,H17,I17,J17,K17,L17,M17,N17,O17,P17,Q17,R17,S17,T17,U17,V17,W17,X17)</f>
+        <v>00000001110000111000000000100100</v>
+      </c>
+      <c r="E17" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>01C38024</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="31" t="str">
+        <f>DEC2BIN(A18,8)</f>
+        <v>00000111</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="N17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="R17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f t="shared" ref="D18:D30" si="1">CONCATENATE(G18,H18,I18,J18,K18,L18,M18,N18,O18,P18,Q18,R18,S18,T18,U18,V18,W18,X18)</f>
+        <v>00000000000101000100000000010010</v>
+      </c>
+      <c r="E18" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>00144012</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="31" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7" t="str">
+      <c r="R18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E19" s="29" t="e">
         <f t="shared" si="0"/>
-        <v>00000000000010000000000000000001</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>6</v>
-      </c>
-      <c r="D17" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>7</v>
-      </c>
-      <c r="D18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D19" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E19" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1527,13 +1716,20 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D20" s="7" t="str">
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>9</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E20" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E20" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1552,17 +1748,27 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D21" s="7" t="str">
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="E21" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E21" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="I21" s="31" t="str">
+        <f>DEC2BIN(A18)</f>
+        <v>111</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1577,13 +1783,20 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D22" s="7" t="str">
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E22" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E22" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1602,13 +1815,20 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D23" s="7" t="str">
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>12</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E23" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E23" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1627,13 +1847,20 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D24" s="7" t="str">
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>13</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E24" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E24" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1652,13 +1879,20 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D25" s="7" t="str">
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>14</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E25" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E25" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1677,13 +1911,20 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D26" s="7" t="str">
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>15</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E26" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E26" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1702,13 +1943,20 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D27" s="7" t="str">
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E27" s="29" t="e">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E27" s="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1727,9 +1975,20 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E28" s="2"/>
+      <c r="X27" s="2"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E28" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1748,9 +2007,20 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E29" s="2"/>
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>18</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E29" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1769,9 +2039,20 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E30" s="2"/>
+      <c r="X29" s="2"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>19</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E30" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1790,9 +2071,12 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E31" s="2"/>
+      <c r="X30" s="2"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>20</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1811,11 +2095,14 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="F32" s="2"/>
+      <c r="X31" s="2"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>21</v>
+      </c>
       <c r="G32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="H32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1830,11 +2117,14 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-    </row>
-    <row r="33" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F33" s="2"/>
+      <c r="X32" s="2"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>22</v>
+      </c>
       <c r="G33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="H33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1849,11 +2139,14 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-    </row>
-    <row r="34" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F34" s="2"/>
+      <c r="X33" s="2"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>23</v>
+      </c>
       <c r="G34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="H34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1868,11 +2161,14 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
-    </row>
-    <row r="35" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F35" s="2"/>
+      <c r="X34" s="2"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>24</v>
+      </c>
       <c r="G35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="H35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1887,11 +2183,11 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
-    </row>
-    <row r="36" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F36" s="2"/>
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="H36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -1906,11 +2202,11 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-    </row>
-    <row r="37" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F37" s="2"/>
+      <c r="X36" s="2"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="H37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -1925,11 +2221,11 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
-    </row>
-    <row r="38" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F38" s="2"/>
+      <c r="X37" s="2"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="H38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -1944,11 +2240,11 @@
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
-    </row>
-    <row r="39" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F39" s="2"/>
+      <c r="X38" s="2"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="H39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1963,11 +2259,11 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
-    </row>
-    <row r="40" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F40" s="2"/>
+      <c r="X39" s="2"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="H40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1982,11 +2278,11 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
-    </row>
-    <row r="41" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F41" s="2"/>
+      <c r="X40" s="2"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="H41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2001,11 +2297,11 @@
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
-    </row>
-    <row r="42" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F42" s="2"/>
+      <c r="X41" s="2"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="H42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2020,11 +2316,11 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
-    </row>
-    <row r="43" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F43" s="2"/>
+      <c r="X42" s="2"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="H43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2039,11 +2335,11 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
-    </row>
-    <row r="44" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F44" s="2"/>
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="H44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2058,11 +2354,11 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
-    </row>
-    <row r="45" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F45" s="2"/>
+      <c r="X44" s="2"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="H45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -2077,11 +2373,11 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
-    </row>
-    <row r="46" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F46" s="2"/>
+      <c r="X45" s="2"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="H46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -2096,11 +2392,11 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
-    </row>
-    <row r="47" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F47" s="2"/>
+      <c r="X46" s="2"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="H47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2115,11 +2411,11 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
-    </row>
-    <row r="48" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F48" s="2"/>
+      <c r="X47" s="2"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G48" s="2"/>
-      <c r="I48" s="2"/>
+      <c r="H48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2134,11 +2430,11 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
-    </row>
-    <row r="49" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F49" s="2"/>
+      <c r="X48" s="2"/>
+    </row>
+    <row r="49" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="H49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2153,11 +2449,11 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
-    </row>
-    <row r="50" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F50" s="2"/>
+      <c r="X49" s="2"/>
+    </row>
+    <row r="50" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G50" s="2"/>
-      <c r="I50" s="2"/>
+      <c r="H50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -2172,11 +2468,11 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
-    </row>
-    <row r="51" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F51" s="2"/>
+      <c r="X50" s="2"/>
+    </row>
+    <row r="51" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="H51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -2191,11 +2487,11 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
-    </row>
-    <row r="52" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F52" s="2"/>
+      <c r="X51" s="2"/>
+    </row>
+    <row r="52" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G52" s="2"/>
-      <c r="I52" s="2"/>
+      <c r="H52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -2210,11 +2506,11 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
-    </row>
-    <row r="53" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F53" s="2"/>
+      <c r="X52" s="2"/>
+    </row>
+    <row r="53" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="H53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -2229,11 +2525,11 @@
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
-    </row>
-    <row r="54" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F54" s="2"/>
+      <c r="X53" s="2"/>
+    </row>
+    <row r="54" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="H54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -2248,11 +2544,11 @@
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
-    </row>
-    <row r="55" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F55" s="2"/>
+      <c r="X54" s="2"/>
+    </row>
+    <row r="55" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G55" s="2"/>
-      <c r="I55" s="2"/>
+      <c r="H55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -2267,11 +2563,11 @@
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
-    </row>
-    <row r="56" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F56" s="2"/>
+      <c r="X55" s="2"/>
+    </row>
+    <row r="56" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G56" s="2"/>
-      <c r="I56" s="2"/>
+      <c r="H56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2286,11 +2582,11 @@
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
-    </row>
-    <row r="57" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F57" s="2"/>
+      <c r="X56" s="2"/>
+    </row>
+    <row r="57" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G57" s="2"/>
-      <c r="I57" s="2"/>
+      <c r="H57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -2305,11 +2601,11 @@
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
       <c r="W57" s="2"/>
-    </row>
-    <row r="58" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F58" s="2"/>
+      <c r="X57" s="2"/>
+    </row>
+    <row r="58" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G58" s="2"/>
-      <c r="I58" s="2"/>
+      <c r="H58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
@@ -2324,11 +2620,11 @@
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
-    </row>
-    <row r="59" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F59" s="2"/>
+      <c r="X58" s="2"/>
+    </row>
+    <row r="59" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G59" s="2"/>
-      <c r="I59" s="2"/>
+      <c r="H59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -2343,11 +2639,11 @@
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
-    </row>
-    <row r="60" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F60" s="2"/>
+      <c r="X59" s="2"/>
+    </row>
+    <row r="60" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="H60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -2362,11 +2658,11 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
-    </row>
-    <row r="61" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F61" s="2"/>
+      <c r="X60" s="2"/>
+    </row>
+    <row r="61" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G61" s="2"/>
-      <c r="I61" s="2"/>
+      <c r="H61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
@@ -2381,11 +2677,11 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
-    </row>
-    <row r="62" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F62" s="2"/>
+      <c r="X61" s="2"/>
+    </row>
+    <row r="62" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G62" s="2"/>
-      <c r="I62" s="2"/>
+      <c r="H62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -2400,11 +2696,11 @@
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
-    </row>
-    <row r="63" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F63" s="2"/>
+      <c r="X62" s="2"/>
+    </row>
+    <row r="63" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G63" s="2"/>
-      <c r="I63" s="2"/>
+      <c r="H63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
@@ -2419,11 +2715,11 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
-    </row>
-    <row r="64" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F64" s="2"/>
+      <c r="X63" s="2"/>
+    </row>
+    <row r="64" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="H64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -2438,11 +2734,11 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
-    </row>
-    <row r="65" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F65" s="2"/>
+      <c r="X64" s="2"/>
+    </row>
+    <row r="65" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G65" s="2"/>
-      <c r="I65" s="2"/>
+      <c r="H65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -2457,11 +2753,11 @@
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
-    </row>
-    <row r="66" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F66" s="2"/>
+      <c r="X65" s="2"/>
+    </row>
+    <row r="66" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G66" s="2"/>
-      <c r="I66" s="2"/>
+      <c r="H66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -2476,11 +2772,11 @@
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
-    </row>
-    <row r="67" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F67" s="2"/>
+      <c r="X66" s="2"/>
+    </row>
+    <row r="67" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G67" s="2"/>
-      <c r="I67" s="2"/>
+      <c r="H67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -2495,11 +2791,11 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
-    </row>
-    <row r="68" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F68" s="2"/>
+      <c r="X67" s="2"/>
+    </row>
+    <row r="68" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="H68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
@@ -2514,11 +2810,11 @@
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
-    </row>
-    <row r="69" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F69" s="2"/>
+      <c r="X68" s="2"/>
+    </row>
+    <row r="69" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G69" s="2"/>
-      <c r="I69" s="2"/>
+      <c r="H69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
@@ -2533,11 +2829,11 @@
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
-    </row>
-    <row r="70" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F70" s="2"/>
+      <c r="X69" s="2"/>
+    </row>
+    <row r="70" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G70" s="2"/>
-      <c r="I70" s="2"/>
+      <c r="H70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -2552,11 +2848,11 @@
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
-    </row>
-    <row r="71" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F71" s="2"/>
+      <c r="X70" s="2"/>
+    </row>
+    <row r="71" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G71" s="2"/>
-      <c r="I71" s="2"/>
+      <c r="H71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -2571,11 +2867,11 @@
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
       <c r="W71" s="2"/>
-    </row>
-    <row r="72" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F72" s="2"/>
+      <c r="X71" s="2"/>
+    </row>
+    <row r="72" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G72" s="2"/>
-      <c r="I72" s="2"/>
+      <c r="H72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
@@ -2590,11 +2886,11 @@
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
-    </row>
-    <row r="73" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F73" s="2"/>
+      <c r="X72" s="2"/>
+    </row>
+    <row r="73" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G73" s="2"/>
-      <c r="I73" s="2"/>
+      <c r="H73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
@@ -2609,11 +2905,11 @@
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
-    </row>
-    <row r="74" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F74" s="2"/>
+      <c r="X73" s="2"/>
+    </row>
+    <row r="74" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G74" s="2"/>
-      <c r="I74" s="2"/>
+      <c r="H74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
@@ -2628,11 +2924,11 @@
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
       <c r="W74" s="2"/>
-    </row>
-    <row r="75" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F75" s="2"/>
+      <c r="X74" s="2"/>
+    </row>
+    <row r="75" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G75" s="2"/>
-      <c r="I75" s="2"/>
+      <c r="H75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
@@ -2647,11 +2943,11 @@
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
       <c r="W75" s="2"/>
-    </row>
-    <row r="76" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F76" s="2"/>
+      <c r="X75" s="2"/>
+    </row>
+    <row r="76" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G76" s="2"/>
-      <c r="I76" s="2"/>
+      <c r="H76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
@@ -2666,11 +2962,11 @@
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
-    </row>
-    <row r="77" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F77" s="2"/>
+      <c r="X76" s="2"/>
+    </row>
+    <row r="77" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G77" s="2"/>
-      <c r="I77" s="2"/>
+      <c r="H77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -2685,11 +2981,11 @@
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
-    </row>
-    <row r="78" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F78" s="2"/>
+      <c r="X77" s="2"/>
+    </row>
+    <row r="78" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G78" s="2"/>
-      <c r="I78" s="2"/>
+      <c r="H78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
@@ -2704,11 +3000,11 @@
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
-    </row>
-    <row r="79" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F79" s="2"/>
+      <c r="X78" s="2"/>
+    </row>
+    <row r="79" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G79" s="2"/>
-      <c r="I79" s="2"/>
+      <c r="H79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
@@ -2723,11 +3019,11 @@
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
-    </row>
-    <row r="80" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F80" s="2"/>
+      <c r="X79" s="2"/>
+    </row>
+    <row r="80" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G80" s="2"/>
-      <c r="I80" s="2"/>
+      <c r="H80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
@@ -2742,11 +3038,11 @@
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
-    </row>
-    <row r="81" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F81" s="2"/>
+      <c r="X80" s="2"/>
+    </row>
+    <row r="81" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G81" s="2"/>
-      <c r="I81" s="2"/>
+      <c r="H81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
@@ -2761,11 +3057,11 @@
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
-    </row>
-    <row r="82" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F82" s="2"/>
+      <c r="X81" s="2"/>
+    </row>
+    <row r="82" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G82" s="2"/>
-      <c r="I82" s="2"/>
+      <c r="H82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
@@ -2780,11 +3076,11 @@
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
-    </row>
-    <row r="83" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F83" s="2"/>
+      <c r="X82" s="2"/>
+    </row>
+    <row r="83" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G83" s="2"/>
-      <c r="I83" s="2"/>
+      <c r="H83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
@@ -2799,11 +3095,11 @@
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
-    </row>
-    <row r="84" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F84" s="2"/>
+      <c r="X83" s="2"/>
+    </row>
+    <row r="84" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G84" s="2"/>
-      <c r="I84" s="2"/>
+      <c r="H84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
@@ -2818,11 +3114,11 @@
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
-    </row>
-    <row r="85" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F85" s="2"/>
+      <c r="X84" s="2"/>
+    </row>
+    <row r="85" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G85" s="2"/>
-      <c r="I85" s="2"/>
+      <c r="H85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
@@ -2837,11 +3133,11 @@
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
-    </row>
-    <row r="86" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F86" s="2"/>
+      <c r="X85" s="2"/>
+    </row>
+    <row r="86" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G86" s="2"/>
-      <c r="I86" s="2"/>
+      <c r="H86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
@@ -2856,11 +3152,11 @@
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
-    </row>
-    <row r="87" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F87" s="2"/>
+      <c r="X86" s="2"/>
+    </row>
+    <row r="87" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G87" s="2"/>
-      <c r="I87" s="2"/>
+      <c r="H87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
@@ -2875,11 +3171,11 @@
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
-    </row>
-    <row r="88" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F88" s="2"/>
+      <c r="X87" s="2"/>
+    </row>
+    <row r="88" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="H88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
@@ -2894,11 +3190,11 @@
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
-    </row>
-    <row r="89" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F89" s="2"/>
+      <c r="X88" s="2"/>
+    </row>
+    <row r="89" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="H89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
@@ -2913,11 +3209,11 @@
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
-    </row>
-    <row r="90" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F90" s="2"/>
+      <c r="X89" s="2"/>
+    </row>
+    <row r="90" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G90" s="2"/>
-      <c r="I90" s="2"/>
+      <c r="H90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
@@ -2932,11 +3228,11 @@
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
       <c r="W90" s="2"/>
-    </row>
-    <row r="91" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F91" s="2"/>
+      <c r="X90" s="2"/>
+    </row>
+    <row r="91" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G91" s="2"/>
-      <c r="I91" s="2"/>
+      <c r="H91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
@@ -2951,11 +3247,11 @@
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
       <c r="W91" s="2"/>
-    </row>
-    <row r="92" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F92" s="2"/>
+      <c r="X91" s="2"/>
+    </row>
+    <row r="92" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G92" s="2"/>
-      <c r="I92" s="2"/>
+      <c r="H92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
@@ -2970,11 +3266,11 @@
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
       <c r="W92" s="2"/>
-    </row>
-    <row r="93" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F93" s="2"/>
+      <c r="X92" s="2"/>
+    </row>
+    <row r="93" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G93" s="2"/>
-      <c r="I93" s="2"/>
+      <c r="H93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
@@ -2989,11 +3285,11 @@
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
       <c r="W93" s="2"/>
-    </row>
-    <row r="94" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F94" s="2"/>
+      <c r="X93" s="2"/>
+    </row>
+    <row r="94" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G94" s="2"/>
-      <c r="I94" s="2"/>
+      <c r="H94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
@@ -3008,11 +3304,11 @@
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
-    </row>
-    <row r="95" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F95" s="2"/>
+      <c r="X94" s="2"/>
+    </row>
+    <row r="95" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G95" s="2"/>
-      <c r="I95" s="2"/>
+      <c r="H95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
@@ -3027,11 +3323,11 @@
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
-    </row>
-    <row r="96" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F96" s="2"/>
+      <c r="X95" s="2"/>
+    </row>
+    <row r="96" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G96" s="2"/>
-      <c r="I96" s="2"/>
+      <c r="H96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
@@ -3046,11 +3342,11 @@
       <c r="U96" s="2"/>
       <c r="V96" s="2"/>
       <c r="W96" s="2"/>
-    </row>
-    <row r="97" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F97" s="2"/>
+      <c r="X96" s="2"/>
+    </row>
+    <row r="97" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G97" s="2"/>
-      <c r="I97" s="2"/>
+      <c r="H97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
@@ -3065,11 +3361,11 @@
       <c r="U97" s="2"/>
       <c r="V97" s="2"/>
       <c r="W97" s="2"/>
-    </row>
-    <row r="98" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F98" s="2"/>
+      <c r="X97" s="2"/>
+    </row>
+    <row r="98" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G98" s="2"/>
-      <c r="I98" s="2"/>
+      <c r="H98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
@@ -3084,11 +3380,11 @@
       <c r="U98" s="2"/>
       <c r="V98" s="2"/>
       <c r="W98" s="2"/>
-    </row>
-    <row r="99" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F99" s="2"/>
+      <c r="X98" s="2"/>
+    </row>
+    <row r="99" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G99" s="2"/>
-      <c r="I99" s="2"/>
+      <c r="H99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
@@ -3103,11 +3399,11 @@
       <c r="U99" s="2"/>
       <c r="V99" s="2"/>
       <c r="W99" s="2"/>
-    </row>
-    <row r="100" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F100" s="2"/>
+      <c r="X99" s="2"/>
+    </row>
+    <row r="100" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G100" s="2"/>
-      <c r="I100" s="2"/>
+      <c r="H100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
@@ -3122,11 +3418,11 @@
       <c r="U100" s="2"/>
       <c r="V100" s="2"/>
       <c r="W100" s="2"/>
-    </row>
-    <row r="101" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F101" s="2"/>
+      <c r="X100" s="2"/>
+    </row>
+    <row r="101" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G101" s="2"/>
-      <c r="I101" s="2"/>
+      <c r="H101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
@@ -3141,11 +3437,11 @@
       <c r="U101" s="2"/>
       <c r="V101" s="2"/>
       <c r="W101" s="2"/>
-    </row>
-    <row r="102" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F102" s="2"/>
+      <c r="X101" s="2"/>
+    </row>
+    <row r="102" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G102" s="2"/>
-      <c r="I102" s="2"/>
+      <c r="H102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
@@ -3160,11 +3456,11 @@
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
       <c r="W102" s="2"/>
-    </row>
-    <row r="103" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F103" s="2"/>
+      <c r="X102" s="2"/>
+    </row>
+    <row r="103" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G103" s="2"/>
-      <c r="I103" s="2"/>
+      <c r="H103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
@@ -3179,11 +3475,11 @@
       <c r="U103" s="2"/>
       <c r="V103" s="2"/>
       <c r="W103" s="2"/>
-    </row>
-    <row r="104" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F104" s="2"/>
+      <c r="X103" s="2"/>
+    </row>
+    <row r="104" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G104" s="2"/>
-      <c r="I104" s="2"/>
+      <c r="H104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
@@ -3198,11 +3494,11 @@
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
       <c r="W104" s="2"/>
-    </row>
-    <row r="105" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F105" s="2"/>
+      <c r="X104" s="2"/>
+    </row>
+    <row r="105" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G105" s="2"/>
-      <c r="I105" s="2"/>
+      <c r="H105" s="2"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
@@ -3217,11 +3513,11 @@
       <c r="U105" s="2"/>
       <c r="V105" s="2"/>
       <c r="W105" s="2"/>
-    </row>
-    <row r="106" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F106" s="2"/>
+      <c r="X105" s="2"/>
+    </row>
+    <row r="106" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G106" s="2"/>
-      <c r="I106" s="2"/>
+      <c r="H106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
@@ -3236,11 +3532,11 @@
       <c r="U106" s="2"/>
       <c r="V106" s="2"/>
       <c r="W106" s="2"/>
-    </row>
-    <row r="107" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F107" s="2"/>
+      <c r="X106" s="2"/>
+    </row>
+    <row r="107" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G107" s="2"/>
-      <c r="I107" s="2"/>
+      <c r="H107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
@@ -3255,11 +3551,11 @@
       <c r="U107" s="2"/>
       <c r="V107" s="2"/>
       <c r="W107" s="2"/>
-    </row>
-    <row r="108" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F108" s="2"/>
+      <c r="X107" s="2"/>
+    </row>
+    <row r="108" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G108" s="2"/>
-      <c r="I108" s="2"/>
+      <c r="H108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
@@ -3274,11 +3570,11 @@
       <c r="U108" s="2"/>
       <c r="V108" s="2"/>
       <c r="W108" s="2"/>
-    </row>
-    <row r="109" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F109" s="2"/>
+      <c r="X108" s="2"/>
+    </row>
+    <row r="109" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G109" s="2"/>
-      <c r="I109" s="2"/>
+      <c r="H109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
@@ -3293,11 +3589,11 @@
       <c r="U109" s="2"/>
       <c r="V109" s="2"/>
       <c r="W109" s="2"/>
-    </row>
-    <row r="110" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F110" s="2"/>
+      <c r="X109" s="2"/>
+    </row>
+    <row r="110" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G110" s="2"/>
-      <c r="I110" s="2"/>
+      <c r="H110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
@@ -3312,11 +3608,11 @@
       <c r="U110" s="2"/>
       <c r="V110" s="2"/>
       <c r="W110" s="2"/>
-    </row>
-    <row r="111" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F111" s="2"/>
+      <c r="X110" s="2"/>
+    </row>
+    <row r="111" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G111" s="2"/>
-      <c r="I111" s="2"/>
+      <c r="H111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
@@ -3331,11 +3627,11 @@
       <c r="U111" s="2"/>
       <c r="V111" s="2"/>
       <c r="W111" s="2"/>
-    </row>
-    <row r="112" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F112" s="2"/>
+      <c r="X111" s="2"/>
+    </row>
+    <row r="112" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G112" s="2"/>
-      <c r="I112" s="2"/>
+      <c r="H112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
@@ -3350,11 +3646,11 @@
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
       <c r="W112" s="2"/>
-    </row>
-    <row r="113" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F113" s="2"/>
+      <c r="X112" s="2"/>
+    </row>
+    <row r="113" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G113" s="2"/>
-      <c r="I113" s="2"/>
+      <c r="H113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
@@ -3369,11 +3665,11 @@
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
       <c r="W113" s="2"/>
-    </row>
-    <row r="114" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F114" s="2"/>
+      <c r="X113" s="2"/>
+    </row>
+    <row r="114" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G114" s="2"/>
-      <c r="I114" s="2"/>
+      <c r="H114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
@@ -3388,11 +3684,11 @@
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
       <c r="W114" s="2"/>
-    </row>
-    <row r="115" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F115" s="2"/>
+      <c r="X114" s="2"/>
+    </row>
+    <row r="115" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G115" s="2"/>
-      <c r="I115" s="2"/>
+      <c r="H115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
@@ -3407,11 +3703,11 @@
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
       <c r="W115" s="2"/>
-    </row>
-    <row r="116" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F116" s="2"/>
+      <c r="X115" s="2"/>
+    </row>
+    <row r="116" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G116" s="2"/>
-      <c r="I116" s="2"/>
+      <c r="H116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
@@ -3426,11 +3722,11 @@
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
       <c r="W116" s="2"/>
-    </row>
-    <row r="117" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F117" s="2"/>
+      <c r="X116" s="2"/>
+    </row>
+    <row r="117" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G117" s="2"/>
-      <c r="I117" s="2"/>
+      <c r="H117" s="2"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
@@ -3445,11 +3741,11 @@
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
       <c r="W117" s="2"/>
-    </row>
-    <row r="118" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F118" s="2"/>
+      <c r="X117" s="2"/>
+    </row>
+    <row r="118" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G118" s="2"/>
-      <c r="I118" s="2"/>
+      <c r="H118" s="2"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
@@ -3464,11 +3760,11 @@
       <c r="U118" s="2"/>
       <c r="V118" s="2"/>
       <c r="W118" s="2"/>
-    </row>
-    <row r="119" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F119" s="2"/>
+      <c r="X118" s="2"/>
+    </row>
+    <row r="119" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G119" s="2"/>
-      <c r="I119" s="2"/>
+      <c r="H119" s="2"/>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
@@ -3483,11 +3779,11 @@
       <c r="U119" s="2"/>
       <c r="V119" s="2"/>
       <c r="W119" s="2"/>
-    </row>
-    <row r="120" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F120" s="2"/>
+      <c r="X119" s="2"/>
+    </row>
+    <row r="120" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G120" s="2"/>
-      <c r="I120" s="2"/>
+      <c r="H120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
@@ -3502,11 +3798,11 @@
       <c r="U120" s="2"/>
       <c r="V120" s="2"/>
       <c r="W120" s="2"/>
-    </row>
-    <row r="121" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F121" s="2"/>
+      <c r="X120" s="2"/>
+    </row>
+    <row r="121" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G121" s="2"/>
-      <c r="I121" s="2"/>
+      <c r="H121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
@@ -3521,11 +3817,11 @@
       <c r="U121" s="2"/>
       <c r="V121" s="2"/>
       <c r="W121" s="2"/>
-    </row>
-    <row r="122" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F122" s="2"/>
+      <c r="X121" s="2"/>
+    </row>
+    <row r="122" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G122" s="2"/>
-      <c r="I122" s="2"/>
+      <c r="H122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
@@ -3540,11 +3836,11 @@
       <c r="U122" s="2"/>
       <c r="V122" s="2"/>
       <c r="W122" s="2"/>
-    </row>
-    <row r="123" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F123" s="2"/>
+      <c r="X122" s="2"/>
+    </row>
+    <row r="123" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G123" s="2"/>
-      <c r="I123" s="2"/>
+      <c r="H123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
@@ -3559,11 +3855,11 @@
       <c r="U123" s="2"/>
       <c r="V123" s="2"/>
       <c r="W123" s="2"/>
-    </row>
-    <row r="124" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F124" s="2"/>
+      <c r="X123" s="2"/>
+    </row>
+    <row r="124" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G124" s="2"/>
-      <c r="I124" s="2"/>
+      <c r="H124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
@@ -3578,11 +3874,11 @@
       <c r="U124" s="2"/>
       <c r="V124" s="2"/>
       <c r="W124" s="2"/>
-    </row>
-    <row r="125" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F125" s="2"/>
+      <c r="X124" s="2"/>
+    </row>
+    <row r="125" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G125" s="2"/>
-      <c r="I125" s="2"/>
+      <c r="H125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
@@ -3597,11 +3893,11 @@
       <c r="U125" s="2"/>
       <c r="V125" s="2"/>
       <c r="W125" s="2"/>
-    </row>
-    <row r="126" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F126" s="2"/>
+      <c r="X125" s="2"/>
+    </row>
+    <row r="126" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G126" s="2"/>
-      <c r="I126" s="2"/>
+      <c r="H126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
@@ -3616,11 +3912,11 @@
       <c r="U126" s="2"/>
       <c r="V126" s="2"/>
       <c r="W126" s="2"/>
-    </row>
-    <row r="127" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F127" s="2"/>
+      <c r="X126" s="2"/>
+    </row>
+    <row r="127" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G127" s="2"/>
-      <c r="I127" s="2"/>
+      <c r="H127" s="2"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
@@ -3635,11 +3931,11 @@
       <c r="U127" s="2"/>
       <c r="V127" s="2"/>
       <c r="W127" s="2"/>
-    </row>
-    <row r="128" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F128" s="2"/>
+      <c r="X127" s="2"/>
+    </row>
+    <row r="128" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G128" s="2"/>
-      <c r="I128" s="2"/>
+      <c r="H128" s="2"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
@@ -3654,11 +3950,11 @@
       <c r="U128" s="2"/>
       <c r="V128" s="2"/>
       <c r="W128" s="2"/>
-    </row>
-    <row r="129" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F129" s="2"/>
+      <c r="X128" s="2"/>
+    </row>
+    <row r="129" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G129" s="2"/>
-      <c r="I129" s="2"/>
+      <c r="H129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
@@ -3673,11 +3969,11 @@
       <c r="U129" s="2"/>
       <c r="V129" s="2"/>
       <c r="W129" s="2"/>
-    </row>
-    <row r="130" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F130" s="2"/>
+      <c r="X129" s="2"/>
+    </row>
+    <row r="130" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G130" s="2"/>
-      <c r="I130" s="2"/>
+      <c r="H130" s="2"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
@@ -3692,11 +3988,11 @@
       <c r="U130" s="2"/>
       <c r="V130" s="2"/>
       <c r="W130" s="2"/>
-    </row>
-    <row r="131" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F131" s="2"/>
+      <c r="X130" s="2"/>
+    </row>
+    <row r="131" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G131" s="2"/>
-      <c r="I131" s="2"/>
+      <c r="H131" s="2"/>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
@@ -3711,11 +4007,11 @@
       <c r="U131" s="2"/>
       <c r="V131" s="2"/>
       <c r="W131" s="2"/>
-    </row>
-    <row r="132" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F132" s="2"/>
+      <c r="X131" s="2"/>
+    </row>
+    <row r="132" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G132" s="2"/>
-      <c r="I132" s="2"/>
+      <c r="H132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
@@ -3730,11 +4026,11 @@
       <c r="U132" s="2"/>
       <c r="V132" s="2"/>
       <c r="W132" s="2"/>
-    </row>
-    <row r="133" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F133" s="2"/>
+      <c r="X132" s="2"/>
+    </row>
+    <row r="133" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G133" s="2"/>
-      <c r="I133" s="2"/>
+      <c r="H133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
@@ -3749,11 +4045,11 @@
       <c r="U133" s="2"/>
       <c r="V133" s="2"/>
       <c r="W133" s="2"/>
-    </row>
-    <row r="134" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F134" s="2"/>
+      <c r="X133" s="2"/>
+    </row>
+    <row r="134" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G134" s="2"/>
-      <c r="I134" s="2"/>
+      <c r="H134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
@@ -3768,11 +4064,11 @@
       <c r="U134" s="2"/>
       <c r="V134" s="2"/>
       <c r="W134" s="2"/>
-    </row>
-    <row r="135" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F135" s="2"/>
+      <c r="X134" s="2"/>
+    </row>
+    <row r="135" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G135" s="2"/>
-      <c r="I135" s="2"/>
+      <c r="H135" s="2"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
@@ -3787,11 +4083,11 @@
       <c r="U135" s="2"/>
       <c r="V135" s="2"/>
       <c r="W135" s="2"/>
-    </row>
-    <row r="136" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F136" s="2"/>
+      <c r="X135" s="2"/>
+    </row>
+    <row r="136" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G136" s="2"/>
-      <c r="I136" s="2"/>
+      <c r="H136" s="2"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
@@ -3806,11 +4102,11 @@
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
       <c r="W136" s="2"/>
-    </row>
-    <row r="137" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F137" s="2"/>
+      <c r="X136" s="2"/>
+    </row>
+    <row r="137" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G137" s="2"/>
-      <c r="I137" s="2"/>
+      <c r="H137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
@@ -3825,11 +4121,11 @@
       <c r="U137" s="2"/>
       <c r="V137" s="2"/>
       <c r="W137" s="2"/>
-    </row>
-    <row r="138" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F138" s="2"/>
+      <c r="X137" s="2"/>
+    </row>
+    <row r="138" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G138" s="2"/>
-      <c r="I138" s="2"/>
+      <c r="H138" s="2"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
@@ -3844,11 +4140,11 @@
       <c r="U138" s="2"/>
       <c r="V138" s="2"/>
       <c r="W138" s="2"/>
-    </row>
-    <row r="139" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F139" s="2"/>
+      <c r="X138" s="2"/>
+    </row>
+    <row r="139" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G139" s="2"/>
-      <c r="I139" s="2"/>
+      <c r="H139" s="2"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
       <c r="L139" s="2"/>
@@ -3863,11 +4159,11 @@
       <c r="U139" s="2"/>
       <c r="V139" s="2"/>
       <c r="W139" s="2"/>
-    </row>
-    <row r="140" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F140" s="2"/>
+      <c r="X139" s="2"/>
+    </row>
+    <row r="140" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G140" s="2"/>
-      <c r="I140" s="2"/>
+      <c r="H140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
       <c r="L140" s="2"/>
@@ -3882,11 +4178,11 @@
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
       <c r="W140" s="2"/>
-    </row>
-    <row r="141" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F141" s="2"/>
+      <c r="X140" s="2"/>
+    </row>
+    <row r="141" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G141" s="2"/>
-      <c r="I141" s="2"/>
+      <c r="H141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
       <c r="L141" s="2"/>
@@ -3901,11 +4197,11 @@
       <c r="U141" s="2"/>
       <c r="V141" s="2"/>
       <c r="W141" s="2"/>
-    </row>
-    <row r="142" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F142" s="2"/>
+      <c r="X141" s="2"/>
+    </row>
+    <row r="142" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G142" s="2"/>
-      <c r="I142" s="2"/>
+      <c r="H142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
@@ -3920,11 +4216,11 @@
       <c r="U142" s="2"/>
       <c r="V142" s="2"/>
       <c r="W142" s="2"/>
-    </row>
-    <row r="143" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F143" s="2"/>
+      <c r="X142" s="2"/>
+    </row>
+    <row r="143" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G143" s="2"/>
-      <c r="I143" s="2"/>
+      <c r="H143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
       <c r="L143" s="2"/>
@@ -3939,11 +4235,11 @@
       <c r="U143" s="2"/>
       <c r="V143" s="2"/>
       <c r="W143" s="2"/>
-    </row>
-    <row r="144" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F144" s="2"/>
+      <c r="X143" s="2"/>
+    </row>
+    <row r="144" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G144" s="2"/>
-      <c r="I144" s="2"/>
+      <c r="H144" s="2"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
       <c r="L144" s="2"/>
@@ -3958,11 +4254,11 @@
       <c r="U144" s="2"/>
       <c r="V144" s="2"/>
       <c r="W144" s="2"/>
-    </row>
-    <row r="145" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F145" s="2"/>
+      <c r="X144" s="2"/>
+    </row>
+    <row r="145" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G145" s="2"/>
-      <c r="I145" s="2"/>
+      <c r="H145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
       <c r="L145" s="2"/>
@@ -3977,11 +4273,11 @@
       <c r="U145" s="2"/>
       <c r="V145" s="2"/>
       <c r="W145" s="2"/>
-    </row>
-    <row r="146" spans="6:23" x14ac:dyDescent="0.3">
-      <c r="F146" s="2"/>
+      <c r="X145" s="2"/>
+    </row>
+    <row r="146" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G146" s="2"/>
-      <c r="I146" s="2"/>
+      <c r="H146" s="2"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
@@ -3996,9 +4292,13 @@
       <c r="U146" s="2"/>
       <c r="V146" s="2"/>
       <c r="W146" s="2"/>
+      <c r="X146" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="I16" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all conditional zero branches
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="103">
   <si>
     <t>NextAddressSource</t>
   </si>
@@ -293,6 +293,36 @@
   </si>
   <si>
     <t>(1bit)</t>
+  </si>
+  <si>
+    <t>Brz</t>
+  </si>
+  <si>
+    <t>Brnz</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Brgz</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Brgez</t>
+  </si>
+  <si>
+    <t>Brlz</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Brlez</t>
   </si>
 </sst>
 </file>
@@ -367,7 +397,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -400,7 +432,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -431,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -445,9 +479,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -456,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -769,9 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I27" sqref="I27"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,8 +816,8 @@
     <col min="1" max="2" width="12.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" customWidth="1"/>
     <col min="9" max="9" width="26.5546875" customWidth="1"/>
@@ -801,7 +838,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="16"/>
+      <c r="F1" s="18"/>
       <c r="M1" s="5" t="s">
         <v>62</v>
       </c>
@@ -810,7 +847,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="16"/>
+      <c r="F2" s="18"/>
       <c r="M2" s="5" t="s">
         <v>64</v>
       </c>
@@ -819,7 +856,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="16"/>
+      <c r="F3" s="18"/>
       <c r="M3" s="5" t="s">
         <v>63</v>
       </c>
@@ -828,7 +865,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="16"/>
+      <c r="F4" s="18"/>
       <c r="M4" s="5" t="s">
         <v>76</v>
       </c>
@@ -837,7 +874,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="16"/>
+      <c r="F5" s="18"/>
       <c r="M5" s="5" t="s">
         <v>77</v>
       </c>
@@ -855,7 +892,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="16"/>
+      <c r="F6" s="18"/>
       <c r="M6" s="5" t="s">
         <v>61</v>
       </c>
@@ -873,7 +910,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="16"/>
+      <c r="F7" s="18"/>
       <c r="H7" s="5" t="s">
         <v>57</v>
       </c>
@@ -927,7 +964,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="16"/>
+      <c r="F8" s="18"/>
       <c r="H8" s="5" t="s">
         <v>56</v>
       </c>
@@ -994,7 +1031,7 @@
       <c r="E9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1117,15 +1154,15 @@
         <f>DEC2HEX(A11)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="str">
-        <f>CONCATENATE(H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11,W11,X11,Y11)</f>
-        <v>0000000010000000000000001001100</v>
-      </c>
-      <c r="F11" s="19" t="str">
+        <f>CONCATENATE(H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,U11,V11,W11,X11,Y11)</f>
+        <v>00000000100000000000000010010100</v>
+      </c>
+      <c r="F11" s="21" t="str">
         <f>CONCATENATE(BIN2HEX(VALUE(MID(E11,1, 4))),BIN2HEX(VALUE(MID(E11,5, 4))),BIN2HEX(VALUE(MID(E11,9, 4))),BIN2HEX(VALUE(MID(E11,13, 4))),BIN2HEX(VALUE(MID(E11,17, 4))),BIN2HEX(VALUE(MID(E11,21, 4))),BIN2HEX(VALUE(MID(E11,25, 4))),BIN2HEX(VALUE(MID(E11,29, 4))))</f>
         <v>00800094</v>
       </c>
@@ -1135,7 +1172,7 @@
       <c r="H11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="21" t="str">
+      <c r="I11" s="23" t="str">
         <f>DEC2BIN(A12,8)</f>
         <v>00000001</v>
       </c>
@@ -1199,10 +1236,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="str">
-        <f t="shared" ref="E12:E30" si="1">CONCATENATE(H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,U12,W12,X12,Y12)</f>
-        <v>0000000101000000000000000000001</v>
-      </c>
-      <c r="F12" s="19" t="str">
+        <f t="shared" ref="E12:E34" si="1">CONCATENATE(H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,U12,V12,W12,X12,Y12)</f>
+        <v>00000001010000000000000000000001</v>
+      </c>
+      <c r="F12" s="21" t="str">
         <f t="shared" ref="F12:F20" si="2">CONCATENATE(BIN2HEX(VALUE(MID(E12,1, 4))),BIN2HEX(VALUE(MID(E12,5, 4))),BIN2HEX(VALUE(MID(E12,9, 4))),BIN2HEX(VALUE(MID(E12,13, 4))),BIN2HEX(VALUE(MID(E12,17, 4))),BIN2HEX(VALUE(MID(E12,21, 4))),BIN2HEX(VALUE(MID(E12,25, 4))),BIN2HEX(VALUE(MID(E12,29, 4))))</f>
         <v>01400001</v>
       </c>
@@ -1212,7 +1249,7 @@
       <c r="H12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="21" t="str">
+      <c r="I12" s="23" t="str">
         <f>DEC2BIN(A13,8)</f>
         <v>00000010</v>
       </c>
@@ -1265,242 +1302,242 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+    <row r="13" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="str">
+      <c r="B13" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>1000000000000000000000000000000</v>
-      </c>
-      <c r="F13" s="20" t="str">
+        <v>10000000000000000000000000000000</v>
+      </c>
+      <c r="F13" s="21" t="str">
         <f t="shared" si="2"/>
         <v>80000000</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="22" t="str">
+      <c r="I13" s="32" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="13" t="s">
+      <c r="J13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="N13" s="13" t="s">
+      <c r="N13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="R13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="U13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="V13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="W13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="X13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y13" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="R13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
         <v>3</v>
       </c>
-      <c r="B14" s="23" t="str">
+      <c r="B14" s="25" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="25">
         <v>0</v>
       </c>
-      <c r="E14" s="8" t="str">
+      <c r="E14" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0000000110000000000000000000000</v>
-      </c>
-      <c r="F14" s="24" t="str">
+        <v>00000001100000000000000000000000</v>
+      </c>
+      <c r="F14" s="27" t="str">
         <f t="shared" si="2"/>
         <v>01800000</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="28">
         <v>0</v>
       </c>
-      <c r="H14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="26" t="str">
+      <c r="H14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="29" t="str">
         <f>DEC2BIN($A$14,8)</f>
         <v>00000011</v>
       </c>
-      <c r="J14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="25" t="s">
+      <c r="J14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="25" t="s">
+      <c r="N14" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="O14" s="25" t="s">
+      <c r="O14" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="P14" s="25" t="s">
+      <c r="P14" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="25" t="s">
+      <c r="Q14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="R14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="S14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X14" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y14" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
+      <c r="R14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y14" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
         <v>4</v>
       </c>
-      <c r="B15" s="23" t="str">
+      <c r="B15" s="25" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="25">
         <v>2</v>
       </c>
-      <c r="E15" s="8" t="str">
+      <c r="E15" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0000001010000111000000000100100</v>
-      </c>
-      <c r="F15" s="24" t="str">
+        <v>00000010100001110000000001000100</v>
+      </c>
+      <c r="F15" s="27" t="str">
         <f t="shared" si="2"/>
         <v>02870044</v>
       </c>
-      <c r="G15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="26" t="str">
+      <c r="G15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="29" t="str">
         <f>DEC2BIN(A16,8)</f>
         <v>00000101</v>
       </c>
-      <c r="J15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M15" s="25" t="s">
+      <c r="J15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="N15" s="25" t="s">
+      <c r="N15" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="25" t="s">
+      <c r="O15" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="25" t="s">
+      <c r="P15" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q15" s="25" t="s">
+      <c r="Q15" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="R15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="S15" s="25" t="s">
+      <c r="R15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S15" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="T15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W15" s="25" t="s">
+      <c r="T15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W15" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="X15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y15" s="25" t="s">
+      <c r="X15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y15" s="28" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1516,9 +1553,9 @@
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000010000000000000000001</v>
-      </c>
-      <c r="F16" s="19" t="str">
+        <v>00000000000100000000000000000001</v>
+      </c>
+      <c r="F16" s="21" t="str">
         <f t="shared" si="2"/>
         <v>00100001</v>
       </c>
@@ -1528,7 +1565,7 @@
       <c r="H16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="29" t="str">
+      <c r="I16" s="32" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
@@ -1581,84 +1618,84 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+    <row r="17" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
         <v>6</v>
       </c>
-      <c r="B17" s="23" t="str">
+      <c r="B17" s="25" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="25">
         <v>3</v>
       </c>
-      <c r="E17" s="8" t="str">
+      <c r="E17" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0000001110000111000000000100100</v>
-      </c>
-      <c r="F17" s="24" t="str">
+        <v>00000011100001110000000001000100</v>
+      </c>
+      <c r="F17" s="27" t="str">
         <f t="shared" si="2"/>
         <v>03870044</v>
       </c>
-      <c r="G17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="26" t="str">
+      <c r="G17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="29" t="str">
         <f>DEC2BIN(A18,8)</f>
         <v>00000111</v>
       </c>
-      <c r="J17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="25" t="s">
+      <c r="J17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N17" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="O17" s="25" t="s">
+      <c r="O17" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="P17" s="25" t="s">
+      <c r="P17" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="Q17" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="R17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="S17" s="25" t="s">
+      <c r="R17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S17" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="T17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W17" s="25" t="s">
+      <c r="T17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W17" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="X17" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y17" s="25" t="s">
+      <c r="X17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y17" s="28" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1674,9 +1711,9 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000101000100000000010010</v>
-      </c>
-      <c r="F18" s="19" t="str">
+        <v>00000000001010001000000000100010</v>
+      </c>
+      <c r="F18" s="21" t="str">
         <f t="shared" si="2"/>
         <v>00288022</v>
       </c>
@@ -1686,7 +1723,7 @@
       <c r="H18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="29" t="str">
+      <c r="I18" s="32" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
@@ -1739,602 +1776,855 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
+    <row r="19" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
         <v>8</v>
       </c>
-      <c r="B19" s="23" t="str">
+      <c r="B19" s="25" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="25">
         <v>4</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E19" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000011111000000000010000</v>
-      </c>
-      <c r="F19" s="24" t="str">
+        <v>00000000000111110000000000100000</v>
+      </c>
+      <c r="F19" s="27" t="str">
         <f t="shared" si="2"/>
         <v>001F0020</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="26" t="str">
+      <c r="G19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="29" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
-      <c r="J19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" s="25" t="s">
+      <c r="J19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="25" t="s">
+      <c r="M19" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="N19" s="25" t="s">
+      <c r="N19" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="25" t="s">
+      <c r="O19" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="P19" s="25" t="s">
+      <c r="P19" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q19" s="25" t="s">
+      <c r="Q19" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="R19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="T19" s="25" t="s">
+      <c r="R19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="U19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y19" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="U19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y19" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
         <v>9</v>
       </c>
-      <c r="B20" s="23" t="str">
+      <c r="B20" s="12" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="12">
         <v>5</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E20" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000000000001010001000000</v>
-      </c>
-      <c r="F20" s="24" t="str">
+        <v>00000000000000000010100010000000</v>
+      </c>
+      <c r="F20" s="22" t="str">
         <f t="shared" si="2"/>
         <v>00002880</v>
       </c>
-      <c r="G20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="26" t="str">
+      <c r="G20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="24" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
-      <c r="J20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="25" t="s">
+      <c r="J20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="N20" s="25" t="s">
+      <c r="N20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="O20" s="25" t="s">
+      <c r="O20" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="25" t="s">
+      <c r="P20" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="Q20" s="25" t="s">
+      <c r="Q20" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="R20" s="25" t="s">
+      <c r="R20" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="S20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="T20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X20" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y20" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
+      <c r="S20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="X20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y20" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
         <v>10</v>
       </c>
-      <c r="B21" s="23" t="str">
+      <c r="B21" s="12" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="12">
         <v>6</v>
       </c>
-      <c r="E21" s="8" t="str">
+      <c r="E21" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000001000100010001000000</v>
-      </c>
-      <c r="F21" s="24" t="str">
-        <f t="shared" ref="F21:F30" si="3">CONCATENATE(BIN2HEX(VALUE(MID(E21,1, 4))),BIN2HEX(VALUE(MID(E21,5, 4))),BIN2HEX(VALUE(MID(E21,9, 4))),BIN2HEX(VALUE(MID(E21,13, 4))),BIN2HEX(VALUE(MID(E21,17, 4))),BIN2HEX(VALUE(MID(E21,21, 4))),BIN2HEX(VALUE(MID(E21,25, 4))),BIN2HEX(VALUE(MID(E21,29, 4))))</f>
+        <v>00000000000010001000100010000000</v>
+      </c>
+      <c r="F21" s="22" t="str">
+        <f t="shared" ref="F21:F34" si="3">CONCATENATE(BIN2HEX(VALUE(MID(E21,1, 4))),BIN2HEX(VALUE(MID(E21,5, 4))),BIN2HEX(VALUE(MID(E21,9, 4))),BIN2HEX(VALUE(MID(E21,13, 4))),BIN2HEX(VALUE(MID(E21,17, 4))),BIN2HEX(VALUE(MID(E21,21, 4))),BIN2HEX(VALUE(MID(E21,25, 4))),BIN2HEX(VALUE(MID(E21,29, 4))))</f>
         <v>00088880</v>
       </c>
-      <c r="G21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="26" t="str">
+      <c r="G21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="24" t="str">
         <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
-      <c r="J21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M21" s="25" t="s">
+      <c r="J21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="N21" s="25" t="s">
+      <c r="N21" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="O21" s="25" t="s">
+      <c r="O21" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="P21" s="25" t="s">
+      <c r="P21" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="Q21" s="25" t="s">
+      <c r="Q21" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="25" t="s">
+      <c r="R21" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="S21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y21" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
+      <c r="S21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="U21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="V21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="W21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="X21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y21" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
         <v>11</v>
       </c>
-      <c r="B22" s="23" t="str">
+      <c r="B22" s="12" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="12">
         <v>7</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E22" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>00000110000100000000000000000</v>
-      </c>
-      <c r="F22" s="24" t="str">
+        <v>00000100100100000000000000001000</v>
+      </c>
+      <c r="F22" s="22" t="str">
         <f t="shared" si="3"/>
-        <v>06100000</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="26" t="str">
-        <f>DEC2BIN(A23,8)</f>
-        <v>00001100</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" s="25" t="s">
+        <v>04900008</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="24" t="str">
+        <f>DEC2BIN(A20,8)</f>
+        <v>00001001</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="N22" s="25" t="s">
+      <c r="M22" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="25" t="s">
+      <c r="O22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="P22" s="25" t="s">
+      <c r="P22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="Q22" s="25" t="s">
+      <c r="Q22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="R22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="S22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="W22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X22" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="R22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="W22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="X22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y22" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
         <v>12</v>
       </c>
-      <c r="B23" s="7" t="str">
+      <c r="B23" s="25" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="D23" s="7">
+      <c r="C23" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="25">
         <v>8</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="E23" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010101110000000</v>
+      </c>
+      <c r="F23" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082B80</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M23" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N23" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O23" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P23" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q23" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="R23" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y23" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <v>13</v>
+      </c>
+      <c r="B24" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="25">
+        <v>9</v>
+      </c>
+      <c r="E24" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010111010000000</v>
+      </c>
+      <c r="F24" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082E80</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N24" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O24" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P24" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q24" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="R24" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y24" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <v>14</v>
+      </c>
+      <c r="B25" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="25">
+        <v>10</v>
+      </c>
+      <c r="E25" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010100110000000</v>
+      </c>
+      <c r="F25" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082980</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N25" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O25" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P25" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q25" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y25" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <v>15</v>
+      </c>
+      <c r="B26" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="25">
+        <v>11</v>
+      </c>
+      <c r="E26" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010101010000000</v>
+      </c>
+      <c r="F26" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082A80</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N26" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O26" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P26" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y26" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <v>16</v>
+      </c>
+      <c r="B27" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="25">
+        <v>12</v>
+      </c>
+      <c r="E27" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010110110000000</v>
+      </c>
+      <c r="F27" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082D80</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P27" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y27" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <v>17</v>
+      </c>
+      <c r="B28" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="25">
+        <v>13</v>
+      </c>
+      <c r="E28" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000010000010110010000000</v>
+      </c>
+      <c r="F28" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>00082C80</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N28" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O28" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P28" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q28" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="R28" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y28" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <v>18</v>
+      </c>
+      <c r="B29" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25">
+        <v>14</v>
+      </c>
+      <c r="E29" s="26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F23" s="19" t="e">
+      <c r="F29" s="27" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>13</v>
-      </c>
-      <c r="B24" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>D</v>
-      </c>
-      <c r="D24" s="7">
-        <v>9</v>
-      </c>
-      <c r="E24" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F24" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>E</v>
-      </c>
-      <c r="D25" s="7">
-        <v>10</v>
-      </c>
-      <c r="E25" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F25" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>15</v>
-      </c>
-      <c r="B26" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="D26" s="7">
-        <v>11</v>
-      </c>
-      <c r="E26" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F26" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>16</v>
-      </c>
-      <c r="B27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D27" s="7">
-        <v>12</v>
-      </c>
-      <c r="E27" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F27" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>17</v>
-      </c>
-      <c r="B28" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D28" s="7">
-        <v>13</v>
-      </c>
-      <c r="E28" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F28" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
-        <v>18</v>
-      </c>
-      <c r="B29" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D29" s="7">
-        <v>14</v>
-      </c>
-      <c r="E29" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
@@ -2351,7 +2641,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F30" s="19" t="e">
+      <c r="F30" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
@@ -2383,6 +2673,17 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="D31" s="7">
+        <v>16</v>
+      </c>
+      <c r="E31" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F31" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2411,6 +2712,17 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="D32" s="7">
+        <v>17</v>
+      </c>
+      <c r="E32" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F32" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -2437,6 +2749,17 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="D33" s="7">
+        <v>18</v>
+      </c>
+      <c r="E33" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F33" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -2462,6 +2785,17 @@
       <c r="B34" s="7" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
+      </c>
+      <c r="D34" s="7">
+        <v>19</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F34" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H34" s="2"/>
       <c r="J34" s="2"/>

</xml_diff>

<commit_message>
movli and movhi instructions
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="114">
   <si>
     <t>NextAddressSource</t>
   </si>
@@ -283,6 +283,9 @@
     <t>Jmpr</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Jal</t>
   </si>
   <si>
@@ -347,6 +350,12 @@
   </si>
   <si>
     <t>Ble</t>
+  </si>
+  <si>
+    <t>Movli</t>
+  </si>
+  <si>
+    <t>Movhi</t>
   </si>
 </sst>
 </file>
@@ -399,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -484,12 +493,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -523,6 +541,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -831,8 +850,8 @@
   <dimension ref="A1:Y146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="9" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,7 +994,7 @@
         <v>48</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>69</v>
@@ -1102,7 +1121,7 @@
         <v>47</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>68</v>
@@ -1158,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W10" s="5" t="s">
         <v>1</v>
@@ -2052,7 +2071,7 @@
         <v>B</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="12">
         <v>7</v>
@@ -2133,7 +2152,7 @@
         <v>C</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D23" s="25">
         <v>8</v>
@@ -2214,7 +2233,7 @@
         <v>D</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" s="25">
         <v>9</v>
@@ -2259,7 +2278,7 @@
         <v>83</v>
       </c>
       <c r="Q24" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R24" s="28" t="s">
         <v>74</v>
@@ -2295,7 +2314,7 @@
         <v>E</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="25">
         <v>10</v>
@@ -2340,7 +2359,7 @@
         <v>83</v>
       </c>
       <c r="Q25" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R25" s="28" t="s">
         <v>74</v>
@@ -2376,7 +2395,7 @@
         <v>F</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D26" s="25">
         <v>11</v>
@@ -2421,7 +2440,7 @@
         <v>83</v>
       </c>
       <c r="Q26" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R26" s="28" t="s">
         <v>74</v>
@@ -2457,7 +2476,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="25">
         <v>12</v>
@@ -2502,7 +2521,7 @@
         <v>83</v>
       </c>
       <c r="Q27" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R27" s="28" t="s">
         <v>74</v>
@@ -2538,7 +2557,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D28" s="25">
         <v>13</v>
@@ -2619,7 +2638,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="25">
         <v>14</v>
@@ -2652,7 +2671,7 @@
         <v>65</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N29" s="28" t="s">
         <v>83</v>
@@ -2700,7 +2719,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30" s="25">
         <v>15</v>
@@ -2733,7 +2752,7 @@
         <v>65</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N30" s="28" t="s">
         <v>83</v>
@@ -2781,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D31" s="25">
         <v>16</v>
@@ -2862,7 +2881,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D32" s="25">
         <v>17</v>
@@ -2907,7 +2926,7 @@
         <v>79</v>
       </c>
       <c r="Q32" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R32" s="28" t="s">
         <v>74</v>
@@ -2943,7 +2962,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D33" s="25">
         <v>18</v>
@@ -2988,7 +3007,7 @@
         <v>79</v>
       </c>
       <c r="Q33" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R33" s="28" t="s">
         <v>74</v>
@@ -3024,7 +3043,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D34" s="25">
         <v>19</v>
@@ -3069,7 +3088,7 @@
         <v>79</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R34" s="28" t="s">
         <v>74</v>
@@ -3105,7 +3124,7 @@
         <v>18</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D35" s="25">
         <v>20</v>
@@ -3150,7 +3169,7 @@
         <v>79</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R35" s="28" t="s">
         <v>74</v>
@@ -3186,7 +3205,7 @@
         <v>19</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D36" s="25">
         <v>21</v>
@@ -3266,72 +3285,159 @@
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="C37" s="25"/>
+      <c r="C37" s="30" t="s">
+        <v>112</v>
+      </c>
       <c r="D37" s="25">
         <v>22</v>
       </c>
       <c r="E37" s="26" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F37" s="27" t="e">
+        <v>00000000000100110000000000100000</v>
+      </c>
+      <c r="F37" s="27" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
-      <c r="P37" s="28"/>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="28"/>
-      <c r="S37" s="28"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="28"/>
-      <c r="V37" s="28"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="28"/>
-      <c r="Y37" s="28"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
+        <v>00130020</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L37" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="N37" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O37" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="P37" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q37" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="R37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T37" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y37" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
         <v>27</v>
       </c>
-      <c r="B38" s="7" t="str">
+      <c r="B38" s="25" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="D38" s="7">
+      <c r="C38" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="25">
         <v>23</v>
       </c>
-      <c r="E38" s="8" t="str">
+      <c r="E38" s="26" t="str">
         <f>CONCATENATE(H38,I38,J38,K38,L38,M38,N38,O38,P38,Q38,R38,S38,T38,U38,V38,W38,X38,Y38)</f>
-        <v/>
-      </c>
-      <c r="F38" s="21" t="e">
+        <v>00000000000100111000000000100000</v>
+      </c>
+      <c r="F38" s="26" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
+        <v>00138020</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="29" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L38" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="M38" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="N38" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="O38" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="P38" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q38" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="R38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T38" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="X38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y38" s="28" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
@@ -3348,10 +3454,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F39" s="21" t="e">
+      <c r="F39" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G39" s="33"/>
       <c r="H39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -3385,10 +3492,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F40" s="21" t="e">
+      <c r="F40" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G40" s="33"/>
       <c r="H40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -3422,10 +3530,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F41" s="21" t="e">
+      <c r="F41" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G41" s="33"/>
       <c r="H41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -3459,10 +3568,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F42" s="21" t="e">
+      <c r="F42" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G42" s="33"/>
       <c r="H42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -3496,10 +3606,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F43" s="21" t="e">
+      <c r="F43" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G43" s="33"/>
       <c r="H43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -3533,10 +3644,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F44" s="21" t="e">
+      <c r="F44" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G44" s="33"/>
       <c r="H44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -3570,10 +3682,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F45" s="21" t="e">
+      <c r="F45" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G45" s="33"/>
       <c r="H45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3607,10 +3720,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F46" s="21" t="e">
+      <c r="F46" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G46" s="33"/>
       <c r="H46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3644,10 +3758,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F47" s="21" t="e">
+      <c r="F47" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G47" s="33"/>
       <c r="H47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -3681,10 +3796,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F48" s="21" t="e">
+      <c r="F48" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G48" s="33"/>
       <c r="H48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -3718,10 +3834,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F49" s="21" t="e">
+      <c r="F49" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G49" s="33"/>
       <c r="H49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3755,10 +3872,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F50" s="21" t="e">
+      <c r="F50" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G50" s="33"/>
       <c r="H50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3792,10 +3910,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F51" s="21" t="e">
+      <c r="F51" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G51" s="33"/>
       <c r="H51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3829,10 +3948,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F52" s="21" t="e">
+      <c r="F52" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G52" s="33"/>
       <c r="H52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -3866,10 +3986,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F53" s="21" t="e">
+      <c r="F53" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G53" s="33"/>
       <c r="H53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -3903,10 +4024,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F54" s="21" t="e">
+      <c r="F54" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G54" s="33"/>
       <c r="H54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -3940,10 +4062,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F55" s="21" t="e">
+      <c r="F55" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G55" s="33"/>
       <c r="H55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -3977,10 +4100,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F56" s="21" t="e">
+      <c r="F56" s="8" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G56" s="33"/>
       <c r="H56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>

</xml_diff>

<commit_message>
all imediate arithmetic instructions
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="115">
   <si>
     <t>NextAddressSource</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Movhi</t>
+  </si>
+  <si>
+    <t>Subi</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -493,15 +496,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -541,7 +535,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -850,8 +846,8 @@
   <dimension ref="A1:Y146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2159,11 +2155,11 @@
       </c>
       <c r="E23" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010101110000000</v>
+        <v>00000000001010000010101110000000</v>
       </c>
       <c r="F23" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082B80</v>
+        <v>00282B80</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>65</v>
@@ -2179,7 +2175,7 @@
         <v>65</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L23" s="28" t="s">
         <v>65</v>
@@ -2240,11 +2236,11 @@
       </c>
       <c r="E24" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010111010000000</v>
+        <v>00000000001010000010111010000000</v>
       </c>
       <c r="F24" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082E80</v>
+        <v>00282E80</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>65</v>
@@ -2260,7 +2256,7 @@
         <v>65</v>
       </c>
       <c r="K24" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>65</v>
@@ -2321,11 +2317,11 @@
       </c>
       <c r="E25" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010100110000000</v>
+        <v>00000000001010000010100110000000</v>
       </c>
       <c r="F25" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082980</v>
+        <v>00282980</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>65</v>
@@ -2341,7 +2337,7 @@
         <v>65</v>
       </c>
       <c r="K25" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L25" s="28" t="s">
         <v>65</v>
@@ -2402,11 +2398,11 @@
       </c>
       <c r="E26" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010101010000000</v>
+        <v>00000000001010000010101010000000</v>
       </c>
       <c r="F26" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082A80</v>
+        <v>00282A80</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>65</v>
@@ -2422,7 +2418,7 @@
         <v>65</v>
       </c>
       <c r="K26" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L26" s="28" t="s">
         <v>65</v>
@@ -2483,11 +2479,11 @@
       </c>
       <c r="E27" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010110110000000</v>
+        <v>00000000001010000010110110000000</v>
       </c>
       <c r="F27" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082D80</v>
+        <v>00282D80</v>
       </c>
       <c r="G27" s="28" t="s">
         <v>65</v>
@@ -2503,7 +2499,7 @@
         <v>65</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L27" s="28" t="s">
         <v>65</v>
@@ -2564,11 +2560,11 @@
       </c>
       <c r="E28" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010000010110010000000</v>
+        <v>00000000001010000010110010000000</v>
       </c>
       <c r="F28" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>00082C80</v>
+        <v>00282C80</v>
       </c>
       <c r="G28" s="28" t="s">
         <v>65</v>
@@ -2584,7 +2580,7 @@
         <v>65</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L28" s="28" t="s">
         <v>65</v>
@@ -3376,7 +3372,7 @@
         <f>CONCATENATE(H38,I38,J38,K38,L38,M38,N38,O38,P38,Q38,R38,S38,T38,U38,V38,W38,X38,Y38)</f>
         <v>00000000000100111000000000100000</v>
       </c>
-      <c r="F38" s="26" t="str">
+      <c r="F38" s="27" t="str">
         <f t="shared" si="5"/>
         <v>00138020</v>
       </c>
@@ -3439,43 +3435,44 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
+    <row r="39" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25">
         <v>28</v>
       </c>
-      <c r="B39" s="7" t="str">
+      <c r="B39" s="25" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="D39" s="7">
+      <c r="C39" s="25"/>
+      <c r="D39" s="25">
         <v>24</v>
       </c>
-      <c r="E39" s="8" t="str">
+      <c r="E39" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F39" s="8" t="e">
+      <c r="F39" s="27" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G39" s="33"/>
-      <c r="H39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
@@ -3492,11 +3489,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F40" s="8" t="e">
+      <c r="F40" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G40" s="33"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -3530,11 +3527,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F41" s="8" t="e">
+      <c r="F41" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G41" s="33"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -3568,11 +3565,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F42" s="8" t="e">
+      <c r="F42" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G42" s="33"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -3606,11 +3603,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F43" s="8" t="e">
+      <c r="F43" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G43" s="33"/>
+      <c r="G43" s="9"/>
       <c r="H43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -3644,11 +3641,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F44" s="8" t="e">
+      <c r="F44" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G44" s="33"/>
+      <c r="G44" s="9"/>
       <c r="H44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -3682,11 +3679,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F45" s="8" t="e">
+      <c r="F45" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G45" s="33"/>
+      <c r="G45" s="9"/>
       <c r="H45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3720,11 +3717,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F46" s="8" t="e">
+      <c r="F46" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G46" s="33"/>
+      <c r="G46" s="9"/>
       <c r="H46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3743,119 +3740,165 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
+    <row r="47" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
         <v>36</v>
       </c>
-      <c r="B47" s="7" t="str">
+      <c r="B47" s="12" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D47" s="7">
+      <c r="C47" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="12">
         <v>32</v>
       </c>
-      <c r="E47" s="8" t="str">
+      <c r="E47" s="13" t="str">
+        <f>CONCATENATE(H47,I47,J47,K47,L47,M47,N47,O47,P47,Q47,R47,S47,T47,U47,V47,W47,X47,Y47)</f>
+        <v>00000000000101000000000000100000</v>
+      </c>
+      <c r="F47" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>00140020</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I47" s="24" t="str">
+        <f>DEC2BIN($A$11,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L47" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="M47" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="N47" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O47" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="P47" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q47" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="R47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="T47" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="U47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="V47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="W47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="X47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y47" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="25">
+        <v>37</v>
+      </c>
+      <c r="B48" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="25">
+        <v>33</v>
+      </c>
+      <c r="E48" s="26" t="str">
+        <f>CONCATENATE(H48,I48,J48,K48,L48,M48,N48,O48,P48,Q48,R48,S48,T48,U48,V48,W48,X48,Y48)</f>
+        <v/>
+      </c>
+      <c r="F48" s="27" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="28"/>
+      <c r="R48" s="28"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="28"/>
+      <c r="U48" s="28"/>
+      <c r="V48" s="28"/>
+      <c r="W48" s="28"/>
+      <c r="X48" s="28"/>
+      <c r="Y48" s="28"/>
+    </row>
+    <row r="49" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25">
+        <v>38</v>
+      </c>
+      <c r="B49" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25">
+        <v>34</v>
+      </c>
+      <c r="E49" s="26" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F47" s="8" t="e">
+      <c r="F49" s="27" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G47" s="33"/>
-      <c r="H47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="2"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
-        <v>37</v>
-      </c>
-      <c r="B48" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="D48" s="7">
-        <v>33</v>
-      </c>
-      <c r="E48" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F48" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G48" s="33"/>
-      <c r="H48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
-        <v>38</v>
-      </c>
-      <c r="B49" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D49" s="7">
-        <v>34</v>
-      </c>
-      <c r="E49" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F49" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G49" s="33"/>
-      <c r="H49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="O49" s="28"/>
+      <c r="P49" s="28"/>
+      <c r="Q49" s="28"/>
+      <c r="R49" s="28"/>
+      <c r="S49" s="28"/>
+      <c r="T49" s="28"/>
+      <c r="U49" s="28"/>
+      <c r="V49" s="28"/>
+      <c r="W49" s="28"/>
+      <c r="X49" s="28"/>
+      <c r="Y49" s="28"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
@@ -3872,11 +3915,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F50" s="8" t="e">
+      <c r="F50" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G50" s="33"/>
+      <c r="G50" s="9"/>
       <c r="H50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3910,11 +3953,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F51" s="8" t="e">
+      <c r="F51" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G51" s="33"/>
+      <c r="G51" s="9"/>
       <c r="H51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3948,11 +3991,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F52" s="8" t="e">
+      <c r="F52" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G52" s="33"/>
+      <c r="G52" s="9"/>
       <c r="H52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -3986,11 +4029,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F53" s="8" t="e">
+      <c r="F53" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G53" s="33"/>
+      <c r="G53" s="9"/>
       <c r="H53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -4024,11 +4067,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F54" s="8" t="e">
+      <c r="F54" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G54" s="33"/>
+      <c r="G54" s="9"/>
       <c r="H54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -4062,11 +4105,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F55" s="8" t="e">
+      <c r="F55" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G55" s="33"/>
+      <c r="G55" s="9"/>
       <c r="H55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -4100,11 +4143,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F56" s="8" t="e">
+      <c r="F56" s="21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G56" s="33"/>
+      <c r="G56" s="9"/>
       <c r="H56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>

</xml_diff>

<commit_message>
Working cpu with display. Features missing
</commit_message>
<xml_diff>
--- a/logisim/Microcodes Design.xlsx
+++ b/logisim/Microcodes Design.xlsx
@@ -999,8 +999,8 @@
   <dimension ref="A1:Y148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="9" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2146,11 +2146,11 @@
       </c>
       <c r="E21" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>00000000000010001000100010000000</v>
+        <v>00000000001010001000100010000000</v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ref="F21:F34" si="3">CONCATENATE(BIN2HEX(VALUE(MID(E21,1, 4))),BIN2HEX(VALUE(MID(E21,5, 4))),BIN2HEX(VALUE(MID(E21,9, 4))),BIN2HEX(VALUE(MID(E21,13, 4))),BIN2HEX(VALUE(MID(E21,17, 4))),BIN2HEX(VALUE(MID(E21,21, 4))),BIN2HEX(VALUE(MID(E21,25, 4))),BIN2HEX(VALUE(MID(E21,29, 4))))</f>
-        <v>00088880</v>
+        <v>00288880</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>65</v>
@@ -2166,7 +2166,7 @@
         <v>65</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L21" s="14" t="s">
         <v>65</v>
@@ -2321,7 +2321,7 @@
         <v>65</v>
       </c>
       <c r="I23" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" ref="I23:I28" si="4">DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
       <c r="J23" s="28" t="s">
@@ -2402,7 +2402,7 @@
         <v>65</v>
       </c>
       <c r="I24" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="4"/>
         <v>00000000</v>
       </c>
       <c r="J24" s="28" t="s">
@@ -2483,7 +2483,7 @@
         <v>65</v>
       </c>
       <c r="I25" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="4"/>
         <v>00000000</v>
       </c>
       <c r="J25" s="28" t="s">
@@ -2564,7 +2564,7 @@
         <v>65</v>
       </c>
       <c r="I26" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="4"/>
         <v>00000000</v>
       </c>
       <c r="J26" s="28" t="s">
@@ -2645,7 +2645,7 @@
         <v>65</v>
       </c>
       <c r="I27" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="4"/>
         <v>00000000</v>
       </c>
       <c r="J27" s="28" t="s">
@@ -2726,7 +2726,7 @@
         <v>65</v>
       </c>
       <c r="I28" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="4"/>
         <v>00000000</v>
       </c>
       <c r="J28" s="28" t="s">
@@ -2969,7 +2969,7 @@
         <v>65</v>
       </c>
       <c r="I31" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" ref="I31:I38" si="5">DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
       <c r="J31" s="28" t="s">
@@ -3050,7 +3050,7 @@
         <v>65</v>
       </c>
       <c r="I32" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="J32" s="28" t="s">
@@ -3131,7 +3131,7 @@
         <v>65</v>
       </c>
       <c r="I33" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="J33" s="28" t="s">
@@ -3212,7 +3212,7 @@
         <v>65</v>
       </c>
       <c r="I34" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="J34" s="28" t="s">
@@ -3279,11 +3279,11 @@
         <v>20</v>
       </c>
       <c r="E35" s="26" t="str">
-        <f t="shared" ref="E35:E77" si="4">CONCATENATE(H35,I35,J35,K35,L35,M35,N35,O35,P35,Q35,R35,S35,T35,U35,V35,W35,X35,Y35)</f>
+        <f t="shared" ref="E35:E77" si="6">CONCATENATE(H35,I35,J35,K35,L35,M35,N35,O35,P35,Q35,R35,S35,T35,U35,V35,W35,X35,Y35)</f>
         <v>00000000001000000101010110000000</v>
       </c>
       <c r="F35" s="27" t="str">
-        <f t="shared" ref="F35:F89" si="5">CONCATENATE(BIN2HEX(VALUE(MID(E35,1, 4))),BIN2HEX(VALUE(MID(E35,5, 4))),BIN2HEX(VALUE(MID(E35,9, 4))),BIN2HEX(VALUE(MID(E35,13, 4))),BIN2HEX(VALUE(MID(E35,17, 4))),BIN2HEX(VALUE(MID(E35,21, 4))),BIN2HEX(VALUE(MID(E35,25, 4))),BIN2HEX(VALUE(MID(E35,29, 4))))</f>
+        <f t="shared" ref="F35:F89" si="7">CONCATENATE(BIN2HEX(VALUE(MID(E35,1, 4))),BIN2HEX(VALUE(MID(E35,5, 4))),BIN2HEX(VALUE(MID(E35,9, 4))),BIN2HEX(VALUE(MID(E35,13, 4))),BIN2HEX(VALUE(MID(E35,17, 4))),BIN2HEX(VALUE(MID(E35,21, 4))),BIN2HEX(VALUE(MID(E35,25, 4))),BIN2HEX(VALUE(MID(E35,29, 4))))</f>
         <v>00205580</v>
       </c>
       <c r="G35" s="28" t="s">
@@ -3293,7 +3293,7 @@
         <v>65</v>
       </c>
       <c r="I35" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="J35" s="28" t="s">
@@ -3360,21 +3360,21 @@
         <v>21</v>
       </c>
       <c r="E36" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>00000000001000000101010010000000</v>
       </c>
       <c r="F36" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v>00205480</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>00205480</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H36" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I36" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
       <c r="J36" s="28" t="s">
@@ -3441,21 +3441,21 @@
         <v>22</v>
       </c>
       <c r="E37" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>00000000000100110000000000100000</v>
       </c>
       <c r="F37" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v>00130020</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>00130020</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I37" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
       <c r="J37" s="28" t="s">
@@ -3526,17 +3526,17 @@
         <v>00000000000100111000000000100000</v>
       </c>
       <c r="F38" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v>00138020</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>00138020</v>
-      </c>
-      <c r="G38" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H38" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="29" t="str">
-        <f>DEC2BIN($A$11,8)</f>
         <v>00000000</v>
       </c>
       <c r="J38" s="28" t="s">
@@ -3601,11 +3601,11 @@
         <v>24</v>
       </c>
       <c r="E39" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F39" s="27" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G39" s="28"/>
@@ -3639,11 +3639,11 @@
         <v>25</v>
       </c>
       <c r="E40" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F40" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G40" s="9"/>
@@ -3677,11 +3677,11 @@
         <v>26</v>
       </c>
       <c r="E41" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F41" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G41" s="9"/>
@@ -3715,11 +3715,11 @@
         <v>27</v>
       </c>
       <c r="E42" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F42" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G42" s="9"/>
@@ -3753,11 +3753,11 @@
         <v>28</v>
       </c>
       <c r="E43" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F43" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G43" s="9"/>
@@ -3791,11 +3791,11 @@
         <v>29</v>
       </c>
       <c r="E44" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F44" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G44" s="9"/>
@@ -3829,11 +3829,11 @@
         <v>30</v>
       </c>
       <c r="E45" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F45" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G45" s="9"/>
@@ -3867,11 +3867,11 @@
         <v>31</v>
       </c>
       <c r="E46" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F46" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G46" s="9"/>
@@ -3912,7 +3912,7 @@
         <v>00000000000101000000000000100000</v>
       </c>
       <c r="F47" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>00140020</v>
       </c>
       <c r="G47" s="14" t="s">
@@ -3991,7 +3991,7 @@
         <v/>
       </c>
       <c r="F48" s="27" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G48" s="14" t="s">
@@ -4029,11 +4029,11 @@
         <v>34</v>
       </c>
       <c r="E49" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F49" s="27" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G49" s="14" t="s">
@@ -4069,11 +4069,11 @@
         <v>35</v>
       </c>
       <c r="E50" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F50" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G50" s="14" t="s">
@@ -4109,11 +4109,11 @@
         <v>36</v>
       </c>
       <c r="E51" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F51" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G51" s="14" t="s">
@@ -4149,11 +4149,11 @@
         <v>37</v>
       </c>
       <c r="E52" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F52" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G52" s="14" t="s">
@@ -4189,11 +4189,11 @@
         <v>38</v>
       </c>
       <c r="E53" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F53" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G53" s="14" t="s">
@@ -4229,11 +4229,11 @@
         <v>39</v>
       </c>
       <c r="E54" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F54" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G54" s="14" t="s">
@@ -4269,11 +4269,11 @@
         <v>40</v>
       </c>
       <c r="E55" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F55" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G55" s="14" t="s">
@@ -4309,11 +4309,11 @@
         <v>41</v>
       </c>
       <c r="E56" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F56" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G56" s="14" t="s">
@@ -4349,11 +4349,11 @@
         <v>42</v>
       </c>
       <c r="E57" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F57" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G57" s="14" t="s">
@@ -4389,11 +4389,11 @@
         <v>43</v>
       </c>
       <c r="E58" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F58" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G58" s="14" t="s">
@@ -4429,11 +4429,11 @@
         <v>44</v>
       </c>
       <c r="E59" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F59" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="14" t="s">
@@ -4469,11 +4469,11 @@
         <v>45</v>
       </c>
       <c r="E60" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F60" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="14" t="s">
@@ -4509,11 +4509,11 @@
         <v>46</v>
       </c>
       <c r="E61" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F61" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G61" s="14" t="s">
@@ -4549,11 +4549,11 @@
         <v>47</v>
       </c>
       <c r="E62" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F62" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G62" s="14" t="s">
@@ -4589,11 +4589,11 @@
         <v>48</v>
       </c>
       <c r="E63" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F63" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G63" s="14" t="s">
@@ -4629,11 +4629,11 @@
         <v>49</v>
       </c>
       <c r="E64" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F64" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G64" s="14" t="s">
@@ -4669,11 +4669,11 @@
         <v>50</v>
       </c>
       <c r="E65" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F65" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G65" s="14" t="s">
@@ -4709,11 +4709,11 @@
         <v>51</v>
       </c>
       <c r="E66" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F66" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G66" s="14" t="s">
@@ -4749,11 +4749,11 @@
         <v>52</v>
       </c>
       <c r="E67" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F67" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G67" s="14" t="s">
@@ -4789,11 +4789,11 @@
         <v>53</v>
       </c>
       <c r="E68" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F68" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G68" s="14" t="s">
@@ -4829,11 +4829,11 @@
         <v>54</v>
       </c>
       <c r="E69" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F69" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G69" s="14" t="s">
@@ -4869,11 +4869,11 @@
         <v>55</v>
       </c>
       <c r="E70" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F70" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G70" s="14" t="s">
@@ -4909,11 +4909,11 @@
         <v>56</v>
       </c>
       <c r="E71" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F71" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G71" s="14" t="s">
@@ -4949,11 +4949,11 @@
         <v>57</v>
       </c>
       <c r="E72" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F72" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G72" s="14" t="s">
@@ -4989,11 +4989,11 @@
         <v>58</v>
       </c>
       <c r="E73" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F73" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G73" s="14" t="s">
@@ -5029,11 +5029,11 @@
         <v>59</v>
       </c>
       <c r="E74" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F74" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G74" s="14" t="s">
@@ -5069,11 +5069,11 @@
         <v>60</v>
       </c>
       <c r="E75" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F75" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G75" s="14" t="s">
@@ -5102,18 +5102,18 @@
         <v>65</v>
       </c>
       <c r="B76" s="7" t="str">
-        <f t="shared" ref="B76:B89" si="6">DEC2HEX(A76)</f>
+        <f t="shared" ref="B76:B89" si="8">DEC2HEX(A76)</f>
         <v>41</v>
       </c>
       <c r="D76" s="7">
         <v>61</v>
       </c>
       <c r="E76" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F76" s="21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G76" s="28" t="s">
@@ -5142,7 +5142,7 @@
         <v>37</v>
       </c>
       <c r="B77" s="36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="C77" s="37" t="s">
@@ -5152,11 +5152,11 @@
         <v>62</v>
       </c>
       <c r="E77" s="38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>00000000000000000000000000000000</v>
       </c>
       <c r="F77" s="38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>00000000</v>
       </c>
       <c r="G77" s="39" t="s">
@@ -5223,7 +5223,7 @@
         <v>38</v>
       </c>
       <c r="B78" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="C78" s="7"/>
@@ -5235,7 +5235,7 @@
         <v/>
       </c>
       <c r="F78" s="8" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G78" s="33"/>
@@ -5262,7 +5262,7 @@
         <v>39</v>
       </c>
       <c r="B79" s="25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="C79" s="30" t="s">
@@ -5276,7 +5276,7 @@
         <v>00000000000100000000000000100000</v>
       </c>
       <c r="F79" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>00100020</v>
       </c>
       <c r="G79" s="34" t="s">
@@ -5343,12 +5343,12 @@
         <v>40</v>
       </c>
       <c r="B80" s="25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="C80" s="30"/>
       <c r="D80" s="25">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E80" s="26"/>
       <c r="F80" s="26"/>
@@ -5373,15 +5373,17 @@
       <c r="Y80" s="28"/>
     </row>
     <row r="81" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="25">
+      <c r="A81" s="7">
         <v>41</v>
       </c>
-      <c r="B81" s="25" t="str">
-        <f t="shared" si="6"/>
+      <c r="B81" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="C81" s="16"/>
-      <c r="D81" s="7"/>
+      <c r="D81" s="7">
+        <v>77</v>
+      </c>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="33"/>
@@ -5405,15 +5407,17 @@
       <c r="Y81" s="9"/>
     </row>
     <row r="82" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="25">
+      <c r="A82" s="7">
         <v>42</v>
       </c>
-      <c r="B82" s="25" t="str">
-        <f t="shared" si="6"/>
+      <c r="B82" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>2A</v>
       </c>
       <c r="C82" s="16"/>
-      <c r="D82" s="7"/>
+      <c r="D82" s="7">
+        <v>78</v>
+      </c>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="33"/>
@@ -5437,22 +5441,22 @@
       <c r="Y82" s="9"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A83" s="25">
+      <c r="A83" s="7">
         <v>43</v>
       </c>
-      <c r="B83" s="25" t="str">
-        <f t="shared" si="6"/>
+      <c r="B83" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>2B</v>
       </c>
       <c r="D83" s="7">
         <v>79</v>
       </c>
       <c r="E83" s="8" t="str">
-        <f t="shared" ref="E83:E89" si="7">CONCATENATE(H83,I83,J83,K83,L83,M83,N83,O83,P83,Q83,R83,S83,T83,U83,V83,W83,X83,Y83)</f>
+        <f t="shared" ref="E83:E89" si="9">CONCATENATE(H83,I83,J83,K83,L83,M83,N83,O83,P83,Q83,R83,S83,T83,U83,V83,W83,X83,Y83)</f>
         <v/>
       </c>
       <c r="F83" s="8" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="G83" s="33"/>
@@ -5480,7 +5484,7 @@
         <v>44</v>
       </c>
       <c r="B84" s="25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2C</v>
       </c>
       <c r="C84" s="30" t="s">
@@ -5494,7 +5498,7 @@
         <v>00000010100100001000000001000100</v>
       </c>
       <c r="F84" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>02908044</v>
       </c>
       <c r="G84" s="34" t="s">
@@ -5558,22 +5562,24 @@
     </row>
     <row r="85" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="25">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B85" s="25" t="str">
-        <f t="shared" si="6"/>
-        <v>2B</v>
+        <f t="shared" si="8"/>
+        <v>2D</v>
       </c>
       <c r="C85" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="D85" s="25"/>
+      <c r="D85" s="25">
+        <v>81</v>
+      </c>
       <c r="E85" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v>00000011100100001000000001000100</v>
+      </c>
+      <c r="F85" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>00000011100100001000000001000100</v>
-      </c>
-      <c r="F85" s="26" t="str">
-        <f t="shared" si="5"/>
         <v>03908044</v>
       </c>
       <c r="G85" s="34" t="s">
@@ -5635,58 +5641,58 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A86" s="7">
-        <v>44</v>
-      </c>
-      <c r="B86" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>2C</v>
-      </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="8" t="str">
+    <row r="86" spans="1:25" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="25">
+        <v>46</v>
+      </c>
+      <c r="B86" s="25" t="str">
+        <f t="shared" si="8"/>
+        <v>2E</v>
+      </c>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F86" s="26" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F86" s="8" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G86" s="33"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="2"/>
-      <c r="S86" s="2"/>
-      <c r="T86" s="2"/>
-      <c r="U86" s="2"/>
-      <c r="V86" s="2"/>
-      <c r="W86" s="2"/>
-      <c r="X86" s="2"/>
-      <c r="Y86" s="2"/>
+      <c r="G86" s="34"/>
+      <c r="H86" s="28"/>
+      <c r="J86" s="28"/>
+      <c r="K86" s="28"/>
+      <c r="L86" s="28"/>
+      <c r="M86" s="28"/>
+      <c r="N86" s="28"/>
+      <c r="O86" s="28"/>
+      <c r="P86" s="28"/>
+      <c r="Q86" s="28"/>
+      <c r="R86" s="28"/>
+      <c r="S86" s="28"/>
+      <c r="T86" s="28"/>
+      <c r="U86" s="28"/>
+      <c r="V86" s="28"/>
+      <c r="W86" s="28"/>
+      <c r="X86" s="28"/>
+      <c r="Y86" s="28"/>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B87" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>2D</v>
+        <f t="shared" si="8"/>
+        <v>2F</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F87" s="8" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F87" s="8" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G87" s="33"/>
@@ -5710,19 +5716,19 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B88" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>2E</v>
+        <f t="shared" si="8"/>
+        <v>30</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F88" s="8" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F88" s="8" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G88" s="33"/>
@@ -5746,19 +5752,19 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B89" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>2F</v>
+        <f t="shared" si="8"/>
+        <v>31</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F89" s="8" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F89" s="8" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G89" s="33"/>

</xml_diff>